<commit_message>
Compare Chini data (cleaned) and Tarallo model
</commit_message>
<xml_diff>
--- a/01_raw_data/chini-biogas/chini_biogas-data.xlsx
+++ b/01_raw_data/chini-biogas/chini_biogas-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sahar/Documents/methane_letter/01_raw_data/chini-biogas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A223341-7B44-3B49-B9CC-E776CC5B6887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EF3241-4E5F-FF44-BEDD-8788D2D50F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="520" windowWidth="37220" windowHeight="21080" activeTab="4" xr2:uid="{E612D14B-5A41-9848-9237-46E1EE074146}"/>
+    <workbookView xWindow="1180" yWindow="520" windowWidth="28520" windowHeight="21080" activeTab="4" xr2:uid="{E612D14B-5A41-9848-9237-46E1EE074146}"/>
   </bookViews>
   <sheets>
     <sheet name="All data" sheetId="1" r:id="rId1"/>
@@ -4402,7 +4402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5537883D-F731-064B-A7AA-31A70F6608D8}">
   <dimension ref="A1:O151"/>
   <sheetViews>
-    <sheetView topLeftCell="G111" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="N123" sqref="N123"/>
     </sheetView>
   </sheetViews>
@@ -8125,7 +8125,7 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8533,7 +8533,7 @@
         <v>968752.81945900002</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="H12" s="28">
         <f>F12*1000</f>

</xml_diff>

<commit_message>
Plot EugeneOR biogas and flow data
</commit_message>
<xml_diff>
--- a/01_raw_data/chini-biogas/chini_biogas-data.xlsx
+++ b/01_raw_data/chini-biogas/chini_biogas-data.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sahar/Documents/methane_letter/01_raw_data/chini-biogas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EF3241-4E5F-FF44-BEDD-8788D2D50F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8466111D-8EB3-4B4F-95EF-04ABCF91F02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="520" windowWidth="28520" windowHeight="21080" activeTab="4" xr2:uid="{E612D14B-5A41-9848-9237-46E1EE074146}"/>
+    <workbookView xWindow="2080" yWindow="520" windowWidth="31980" windowHeight="21080" activeTab="1" xr2:uid="{E612D14B-5A41-9848-9237-46E1EE074146}"/>
   </bookViews>
   <sheets>
     <sheet name="All data" sheetId="1" r:id="rId1"/>
     <sheet name="Biogas Data" sheetId="2" r:id="rId2"/>
-    <sheet name="Biogas Col Key" sheetId="3" r:id="rId3"/>
-    <sheet name="Unit conversions" sheetId="4" r:id="rId4"/>
-    <sheet name="Plotting" sheetId="5" r:id="rId5"/>
+    <sheet name="Cities with Complete Data" sheetId="6" r:id="rId3"/>
+    <sheet name="Biogas Col Key" sheetId="3" r:id="rId4"/>
+    <sheet name="Unit conversions" sheetId="4" r:id="rId5"/>
+    <sheet name="Plotting" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="402">
   <si>
     <t>CWNS ID</t>
   </si>
@@ -1236,6 +1237,15 @@
   </si>
   <si>
     <t>MMBtu per therm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> influent_2012_MG </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> facility_size_MGD </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> biogas_gen_value </t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1255,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1322,8 +1332,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1334,6 +1358,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1350,7 +1380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1397,7 +1427,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1413,14 +1442,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1434,6 +1456,29 @@
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2008,7 +2053,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2532,6 +2576,9 @@
                 <c:pt idx="28">
                   <c:v>79.581693989071042</c:v>
                 </c:pt>
+                <c:pt idx="30">
+                  <c:v>156.51639344262296</c:v>
+                </c:pt>
                 <c:pt idx="33">
                   <c:v>81.034672131147531</c:v>
                 </c:pt>
@@ -2663,6 +2710,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>338700000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>213348333.33333337</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>132875000</c:v>
@@ -4402,8 +4452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5537883D-F731-064B-A7AA-31A70F6608D8}">
   <dimension ref="A1:O151"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="N123" sqref="N123"/>
+    <sheetView topLeftCell="D70" workbookViewId="0">
+      <selection activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8117,6 +8167,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8124,8 +8175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1169CC32-FE8E-0247-8B6B-8C48D3D455D8}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8133,12 +8184,12 @@
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" style="39" customWidth="1"/>
-    <col min="6" max="6" width="23.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" style="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="21.83203125" style="39" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" style="39" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" style="35" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="21.83203125" style="35" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" style="35" customWidth="1"/>
     <col min="11" max="11" width="21.6640625" customWidth="1"/>
     <col min="12" max="12" width="91.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -8153,25 +8204,25 @@
       <c r="C1" s="14" t="s">
         <v>361</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="32" t="s">
         <v>362</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="32" t="s">
         <v>391</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="32" t="s">
         <v>363</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="32" t="s">
         <v>364</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="32" t="s">
         <v>366</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="32" t="s">
         <v>380</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="32" t="s">
         <v>365</v>
       </c>
       <c r="K1" s="12" t="s">
@@ -8191,22 +8242,22 @@
       <c r="C2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="29">
         <v>20655.689999999999</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="29">
         <f>D2/366</f>
         <v>56.436311475409831</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29">
         <v>7671726</v>
       </c>
       <c r="K2" s="17"/>
@@ -8224,28 +8275,28 @@
       <c r="C3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>12180.388000000001</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="29">
         <f t="shared" ref="E3:E51" si="0">D3/366</f>
         <v>33.279748633879784</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="29">
         <v>137991.37820000001</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="29">
         <f>F3*1000</f>
         <v>137991378.20000002</v>
       </c>
-      <c r="I3" s="30">
-        <f>H3/D3</f>
+      <c r="I3" s="29">
+        <f t="shared" ref="I3:I22" si="1">H3/D3</f>
         <v>11328.980505382917</v>
       </c>
-      <c r="J3" s="37"/>
+      <c r="J3" s="33"/>
       <c r="K3" s="17"/>
     </row>
     <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.2">
@@ -8258,65 +8309,65 @@
       <c r="C4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="28">
         <v>4989.9480000000003</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="29">
         <f t="shared" si="0"/>
         <v>13.633737704918033</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="28">
         <v>59659000</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H4" s="29">
+      <c r="H4" s="28">
         <f>F4</f>
         <v>59659000</v>
       </c>
-      <c r="I4" s="30">
-        <f>H4/D4</f>
+      <c r="I4" s="29">
+        <f t="shared" si="1"/>
         <v>11955.836012719972</v>
       </c>
-      <c r="J4" s="29">
+      <c r="J4" s="28">
         <v>2625292</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
+    <row r="5" spans="1:12" s="26" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="27">
         <f>131.9*366</f>
         <v>48275.4</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="30">
         <f t="shared" si="0"/>
         <v>131.9</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="27">
         <f>10987*366</f>
         <v>4021242</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="27">
         <f>F5*1000</f>
         <v>4021242000</v>
       </c>
-      <c r="I5" s="31">
-        <f>H5/D5</f>
+      <c r="I5" s="30">
+        <f t="shared" si="1"/>
         <v>83297.95299469294</v>
       </c>
-      <c r="J5" s="38"/>
+      <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
@@ -8328,25 +8379,25 @@
       <c r="C6" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="28">
         <v>5515.83</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="29">
         <f t="shared" si="0"/>
         <v>15.070573770491803</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="28">
         <v>86030950</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="28">
         <f>F6</f>
         <v>86030950</v>
       </c>
-      <c r="I6" s="30">
-        <f>H6/D6</f>
+      <c r="I6" s="29">
+        <f t="shared" si="1"/>
         <v>15597.099620546682</v>
       </c>
     </row>
@@ -8360,26 +8411,26 @@
       <c r="C7" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="28">
         <v>4564.37</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <f t="shared" si="0"/>
         <v>12.470956284153004</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="28">
         <f>49347*1000</f>
         <v>49347000</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="28">
         <f>F7</f>
         <v>49347000</v>
       </c>
-      <c r="I7" s="30">
-        <f>H7/D7</f>
+      <c r="I7" s="29">
+        <f t="shared" si="1"/>
         <v>10811.349649568287</v>
       </c>
     </row>
@@ -8393,25 +8444,25 @@
       <c r="C8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="28">
         <v>41314</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="29">
         <f t="shared" si="0"/>
         <v>112.87978142076503</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="28">
         <v>174134200</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="28">
         <f>F8</f>
         <v>174134200</v>
       </c>
-      <c r="I8" s="30">
-        <f>H8/D8</f>
+      <c r="I8" s="29">
+        <f t="shared" si="1"/>
         <v>4214.8956770102141</v>
       </c>
     </row>
@@ -8425,25 +8476,25 @@
       <c r="C9" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="36">
         <v>2921.9</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="29">
         <f t="shared" si="0"/>
         <v>7.9833333333333334</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="28">
         <v>111328</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="28">
         <f>F9*'Unit conversions'!$E$2</f>
         <v>18554666.666666668</v>
       </c>
-      <c r="I9" s="29">
-        <f>H9/D9</f>
+      <c r="I9" s="28">
+        <f t="shared" si="1"/>
         <v>6350.2059162417154</v>
       </c>
     </row>
@@ -8457,94 +8508,94 @@
       <c r="C10" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="36">
         <v>8681.7999999999993</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="29">
         <f t="shared" si="0"/>
         <v>23.720765027322404</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="28">
         <v>457588</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="28">
         <f>F10*'Unit conversions'!$E$2</f>
         <v>76264666.666666672</v>
       </c>
-      <c r="I10" s="29">
-        <f>H10/D10</f>
+      <c r="I10" s="28">
+        <f t="shared" si="1"/>
         <v>8784.430264077344</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="35" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D11" s="37">
         <v>224980</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="38">
         <f t="shared" si="0"/>
         <v>614.6994535519126</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F11" s="31">
         <v>1093162</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="34">
+      <c r="H11" s="31">
         <f>F11*'Unit conversions'!$E$2</f>
         <v>182193666.66666669</v>
       </c>
-      <c r="I11" s="34">
-        <f>H11/D11</f>
+      <c r="I11" s="31">
+        <f t="shared" si="1"/>
         <v>809.82161377307625</v>
       </c>
-      <c r="J11" s="43"/>
-    </row>
-    <row r="12" spans="1:12" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+      <c r="J11" s="39"/>
+    </row>
+    <row r="12" spans="1:12" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="27">
         <v>45980.601474900002</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="30">
         <f t="shared" si="0"/>
         <v>125.63005867459017</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="27">
         <v>968752.81945900002</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="27">
         <f>F12*1000</f>
         <v>968752819.45899999</v>
       </c>
-      <c r="I12" s="28">
-        <f>H12/D12</f>
+      <c r="I12" s="27">
+        <f t="shared" si="1"/>
         <v>21068.728733090302</v>
       </c>
-      <c r="J12" s="38"/>
-      <c r="L12" s="27" t="s">
+      <c r="J12" s="34"/>
+      <c r="L12" s="26" t="s">
         <v>392</v>
       </c>
     </row>
@@ -8558,25 +8609,25 @@
       <c r="C13" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="28">
         <v>13070.65</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="29">
         <f t="shared" si="0"/>
         <v>35.712158469945351</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="28">
         <v>206329392</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="29">
-        <f>F13</f>
+      <c r="H13" s="28">
+        <f t="shared" ref="H13:H18" si="2">F13</f>
         <v>206329392</v>
       </c>
-      <c r="I13" s="29">
-        <f>H13/D13</f>
+      <c r="I13" s="28">
+        <f t="shared" si="1"/>
         <v>15785.702470802906</v>
       </c>
     </row>
@@ -8590,26 +8641,26 @@
       <c r="C14" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="28">
         <v>10486.9</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="29">
         <f t="shared" si="0"/>
         <v>28.652732240437157</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="28">
         <f>331670*366</f>
         <v>121391220</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H14" s="29">
-        <f>F14</f>
+      <c r="H14" s="28">
+        <f t="shared" si="2"/>
         <v>121391220</v>
       </c>
-      <c r="I14" s="29">
-        <f>H14/D14</f>
+      <c r="I14" s="28">
+        <f t="shared" si="1"/>
         <v>11575.510398687888</v>
       </c>
     </row>
@@ -8623,26 +8674,26 @@
       <c r="C15" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="28">
         <v>6945.31</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="29">
         <f t="shared" si="0"/>
         <v>18.976256830601095</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="28">
         <f>214939*366</f>
         <v>78667674</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H15" s="29">
-        <f>F15</f>
+      <c r="H15" s="28">
+        <f t="shared" si="2"/>
         <v>78667674</v>
       </c>
-      <c r="I15" s="29">
-        <f>H15/D15</f>
+      <c r="I15" s="28">
+        <f t="shared" si="1"/>
         <v>11326.73329196249</v>
       </c>
     </row>
@@ -8656,26 +8707,26 @@
       <c r="C16" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="28">
         <v>2321.3200000000002</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="29">
         <f t="shared" si="0"/>
         <v>6.3424043715847001</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F16" s="28">
         <f>81095*366</f>
         <v>29680770</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H16" s="29">
-        <f>F16</f>
+      <c r="H16" s="28">
+        <f t="shared" si="2"/>
         <v>29680770</v>
       </c>
-      <c r="I16" s="29">
-        <f>H16/D16</f>
+      <c r="I16" s="28">
+        <f t="shared" si="1"/>
         <v>12786.160460427687</v>
       </c>
     </row>
@@ -8689,25 +8740,25 @@
       <c r="C17" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="28">
         <v>15202.37097</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="29">
         <f t="shared" si="0"/>
         <v>41.536532704918031</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="28">
         <v>159260997.59999999</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="G17" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H17" s="29">
-        <f>F17</f>
+      <c r="H17" s="28">
+        <f t="shared" si="2"/>
         <v>159260997.59999999</v>
       </c>
-      <c r="I17" s="29">
-        <f>H17/D17</f>
+      <c r="I17" s="28">
+        <f t="shared" si="1"/>
         <v>10476.063103201592</v>
       </c>
     </row>
@@ -8721,25 +8772,25 @@
       <c r="C18" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="28">
         <v>4388.5749999999998</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E18" s="29">
         <f t="shared" si="0"/>
         <v>11.990642076502732</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="28">
         <v>51331878</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="G18" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H18" s="29">
-        <f>F18</f>
+      <c r="H18" s="28">
+        <f t="shared" si="2"/>
         <v>51331878</v>
       </c>
-      <c r="I18" s="29">
-        <f>H18/D18</f>
+      <c r="I18" s="28">
+        <f t="shared" si="1"/>
         <v>11696.70747338259</v>
       </c>
     </row>
@@ -8753,25 +8804,25 @@
       <c r="C19" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="28">
         <v>17185.400000000001</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="29">
         <f t="shared" si="0"/>
         <v>46.954644808743176</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="28">
         <v>284977.5</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="G19" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="H19" s="29">
+      <c r="H19" s="28">
         <f>F19*1000</f>
         <v>284977500</v>
       </c>
-      <c r="I19" s="29">
-        <f>H19/D19</f>
+      <c r="I19" s="28">
+        <f t="shared" si="1"/>
         <v>16582.53517520686</v>
       </c>
     </row>
@@ -8785,25 +8836,25 @@
       <c r="C20" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="28">
         <v>549.65</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="29">
         <f t="shared" si="0"/>
         <v>1.5017759562841528</v>
       </c>
-      <c r="F20" s="29">
+      <c r="F20" s="28">
         <v>3709528</v>
       </c>
-      <c r="G20" s="29" t="s">
+      <c r="G20" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H20" s="29">
+      <c r="H20" s="28">
         <f>F20</f>
         <v>3709528</v>
       </c>
-      <c r="I20" s="29">
-        <f>H20/D20</f>
+      <c r="I20" s="28">
+        <f t="shared" si="1"/>
         <v>6748.8911125261529</v>
       </c>
       <c r="K20" s="3" t="s">
@@ -8820,25 +8871,25 @@
       <c r="C21" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="D21" s="29">
+      <c r="D21" s="28">
         <v>1374.44</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E21" s="29">
         <f t="shared" si="0"/>
         <v>3.7553005464480878</v>
       </c>
-      <c r="F21" s="29">
+      <c r="F21" s="28">
         <v>22284115</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="G21" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H21" s="29">
+      <c r="H21" s="28">
         <f>F21</f>
         <v>22284115</v>
       </c>
-      <c r="I21" s="29">
-        <f>H21/D21</f>
+      <c r="I21" s="28">
+        <f t="shared" si="1"/>
         <v>16213.232298245102</v>
       </c>
       <c r="K21" s="3" t="s">
@@ -8855,25 +8906,25 @@
       <c r="C22" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="28">
         <v>1932.74</v>
       </c>
-      <c r="E22" s="30">
+      <c r="E22" s="29">
         <f t="shared" si="0"/>
         <v>5.2807103825136616</v>
       </c>
-      <c r="F22" s="29">
+      <c r="F22" s="28">
         <v>38351800</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="G22" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H22" s="29">
+      <c r="H22" s="28">
         <f>F22</f>
         <v>38351800</v>
       </c>
-      <c r="I22" s="29">
-        <f>H22/D22</f>
+      <c r="I22" s="28">
+        <f t="shared" si="1"/>
         <v>19843.227749205791</v>
       </c>
       <c r="K22" s="3" t="s">
@@ -8890,20 +8941,20 @@
       <c r="C23" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E23" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="28">
         <v>12294363</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="G23" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H23" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="I23" s="29"/>
+      <c r="H23" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="I23" s="28"/>
       <c r="K23" s="3" t="s">
         <v>393</v>
       </c>
@@ -8918,25 +8969,25 @@
       <c r="C24" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="28">
         <v>14426.1</v>
       </c>
-      <c r="E24" s="30">
+      <c r="E24" s="29">
         <f t="shared" si="0"/>
         <v>39.415573770491804</v>
       </c>
-      <c r="F24" s="29">
+      <c r="F24" s="28">
         <v>236718970</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H24" s="29">
+      <c r="H24" s="28">
         <f>F24</f>
         <v>236718970</v>
       </c>
-      <c r="I24" s="29">
-        <f>H24/D24</f>
+      <c r="I24" s="28">
+        <f t="shared" ref="I24:I32" si="3">H24/D24</f>
         <v>16409.075911022384</v>
       </c>
     </row>
@@ -8950,28 +9001,28 @@
       <c r="C25" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D25" s="29">
+      <c r="D25" s="28">
         <v>8699.5897199999999</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="29">
         <f t="shared" si="0"/>
         <v>23.76937081967213</v>
       </c>
-      <c r="F25" s="29">
+      <c r="F25" s="28">
         <v>133967709.40000001</v>
       </c>
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H25" s="29">
+      <c r="H25" s="28">
         <f>F25</f>
         <v>133967709.40000001</v>
       </c>
-      <c r="I25" s="29">
-        <f>H25/D25</f>
+      <c r="I25" s="28">
+        <f t="shared" si="3"/>
         <v>15399.313497740444</v>
       </c>
-      <c r="J25" s="29">
+      <c r="J25" s="28">
         <v>5611341</v>
       </c>
       <c r="K25" s="3" t="s">
@@ -8988,28 +9039,28 @@
       <c r="C26" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="28">
         <v>823.02873199999999</v>
       </c>
-      <c r="E26" s="30">
+      <c r="E26" s="29">
         <f t="shared" si="0"/>
         <v>2.248712382513661</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F26" s="28">
         <v>6468208.7000000002</v>
       </c>
-      <c r="G26" s="29" t="s">
+      <c r="G26" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H26" s="29">
+      <c r="H26" s="28">
         <f>F26</f>
         <v>6468208.7000000002</v>
       </c>
-      <c r="I26" s="29">
-        <f>H26/D26</f>
+      <c r="I26" s="28">
+        <f t="shared" si="3"/>
         <v>7859.0314633146982</v>
       </c>
-      <c r="J26" s="29" t="s">
+      <c r="J26" s="28" t="s">
         <v>177</v>
       </c>
       <c r="K26" s="3" t="s">
@@ -9026,25 +9077,25 @@
       <c r="C27" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D27" s="29">
+      <c r="D27" s="28">
         <v>38173.980000000003</v>
       </c>
-      <c r="E27" s="30">
+      <c r="E27" s="29">
         <f t="shared" si="0"/>
         <v>104.3004918032787</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="28">
         <v>415332388.10000002</v>
       </c>
-      <c r="G27" s="29" t="s">
+      <c r="G27" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H27" s="29">
+      <c r="H27" s="28">
         <f>F27</f>
         <v>415332388.10000002</v>
       </c>
-      <c r="I27" s="29">
-        <f>H27/D27</f>
+      <c r="I27" s="28">
+        <f t="shared" si="3"/>
         <v>10879.986527472378</v>
       </c>
     </row>
@@ -9058,25 +9109,25 @@
       <c r="C28" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="28">
         <v>13410.743</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="29">
         <f t="shared" si="0"/>
         <v>36.641374316939888</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="28">
         <v>331468584.19999999</v>
       </c>
-      <c r="G28" s="29" t="s">
+      <c r="G28" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H28" s="29">
+      <c r="H28" s="28">
         <f>F28</f>
         <v>331468584.19999999</v>
       </c>
-      <c r="I28" s="29">
-        <f>H28/D28</f>
+      <c r="I28" s="28">
+        <f t="shared" si="3"/>
         <v>24716.645766755799</v>
       </c>
     </row>
@@ -9090,25 +9141,25 @@
       <c r="C29" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="28">
         <v>13420</v>
       </c>
-      <c r="E29" s="30">
+      <c r="E29" s="29">
         <f t="shared" si="0"/>
         <v>36.666666666666664</v>
       </c>
-      <c r="F29" s="29">
+      <c r="F29" s="28">
         <v>331.36</v>
       </c>
-      <c r="G29" s="29" t="s">
+      <c r="G29" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="H29" s="29">
+      <c r="H29" s="28">
         <f>F29*1000000</f>
         <v>331360000</v>
       </c>
-      <c r="I29" s="29">
-        <f>H29/D29</f>
+      <c r="I29" s="28">
+        <f t="shared" si="3"/>
         <v>24691.505216095378</v>
       </c>
     </row>
@@ -9122,94 +9173,94 @@
       <c r="C30" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D30" s="29">
+      <c r="D30" s="28">
         <v>29126.9</v>
       </c>
-      <c r="E30" s="30">
+      <c r="E30" s="29">
         <f t="shared" si="0"/>
         <v>79.581693989071042</v>
       </c>
-      <c r="F30" s="29">
+      <c r="F30" s="28">
         <v>338700000</v>
       </c>
-      <c r="G30" s="29" t="s">
+      <c r="G30" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H30" s="29">
+      <c r="H30" s="28">
         <f>F30</f>
         <v>338700000</v>
       </c>
-      <c r="I30" s="29">
-        <f>H30/D30</f>
+      <c r="I30" s="28">
+        <f t="shared" si="3"/>
         <v>11628.425956761619</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A31" s="24" t="s">
+    <row r="31" spans="1:11" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A31" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="D31" s="28">
+      <c r="D31" s="27">
         <v>24848.799999999999</v>
       </c>
-      <c r="E31" s="31">
+      <c r="E31" s="30">
         <f t="shared" si="0"/>
         <v>67.892896174863381</v>
       </c>
-      <c r="F31" s="28">
+      <c r="F31" s="27">
         <v>1085100000</v>
       </c>
-      <c r="G31" s="28" t="s">
+      <c r="G31" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="H31" s="28">
+      <c r="H31" s="27">
         <f>F31</f>
         <v>1085100000</v>
       </c>
-      <c r="I31" s="28">
-        <f>H31/D31</f>
+      <c r="I31" s="27">
+        <f t="shared" si="3"/>
         <v>43668.104697208721</v>
       </c>
-      <c r="J31" s="38"/>
-    </row>
-    <row r="32" spans="1:11" s="27" customFormat="1" ht="105" x14ac:dyDescent="0.2">
-      <c r="A32" s="24" t="s">
+      <c r="J31" s="34"/>
+    </row>
+    <row r="32" spans="1:11" s="26" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A32" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="D32" s="28">
+      <c r="D32" s="27">
         <v>57285</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="30">
         <f t="shared" si="0"/>
         <v>156.51639344262296</v>
       </c>
-      <c r="F32" s="28">
+      <c r="F32" s="27">
         <v>128009</v>
       </c>
-      <c r="G32" s="28" t="s">
+      <c r="G32" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="H32" s="28">
+      <c r="H32" s="27">
         <f>F32*'Unit conversions'!E2*10</f>
         <v>213348333.33333337</v>
       </c>
-      <c r="I32" s="28">
-        <f>H32/D32</f>
+      <c r="I32" s="27">
+        <f t="shared" si="3"/>
         <v>3724.331558581363</v>
       </c>
-      <c r="J32" s="38"/>
-      <c r="K32" s="25" t="s">
+      <c r="J32" s="34"/>
+      <c r="K32" s="24" t="s">
         <v>205</v>
       </c>
     </row>
@@ -9223,20 +9274,20 @@
       <c r="C33" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="E33" s="30">
+      <c r="E33" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F33" s="29">
+      <c r="F33" s="28">
         <v>125360687</v>
       </c>
-      <c r="G33" s="29" t="s">
+      <c r="G33" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H33" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="I33" s="29"/>
+      <c r="H33" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="I33" s="28"/>
       <c r="K33" t="s">
         <v>393</v>
       </c>
@@ -9251,25 +9302,25 @@
       <c r="C34" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D34" s="29">
+      <c r="D34" s="28">
         <v>25594</v>
       </c>
-      <c r="E34" s="30">
+      <c r="E34" s="29">
         <f t="shared" si="0"/>
         <v>69.928961748633881</v>
       </c>
-      <c r="F34" s="29">
+      <c r="F34" s="28">
         <v>1072223</v>
       </c>
-      <c r="G34" s="29" t="s">
+      <c r="G34" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="H34" s="29">
+      <c r="H34" s="28">
         <f>F34*1000</f>
         <v>1072223000</v>
       </c>
-      <c r="I34" s="29">
-        <f>H34/D34</f>
+      <c r="I34" s="28">
+        <f t="shared" ref="I34:I51" si="4">H34/D34</f>
         <v>41893.529733531293</v>
       </c>
       <c r="K34" t="s">
@@ -9286,28 +9337,28 @@
       <c r="C35" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="D35" s="29">
+      <c r="D35" s="28">
         <v>29658.69</v>
       </c>
-      <c r="E35" s="30">
+      <c r="E35" s="29">
         <f t="shared" si="0"/>
         <v>81.034672131147531</v>
       </c>
-      <c r="F35" s="44">
+      <c r="F35" s="40">
         <v>132.875</v>
       </c>
-      <c r="G35" s="29" t="s">
+      <c r="G35" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="H35" s="29">
+      <c r="H35" s="28">
         <f>F35*1000000</f>
         <v>132875000</v>
       </c>
-      <c r="I35" s="29">
-        <f>H35/D35</f>
+      <c r="I35" s="28">
+        <f t="shared" si="4"/>
         <v>4480.1371874482656</v>
       </c>
-      <c r="J35" s="29" t="s">
+      <c r="J35" s="28" t="s">
         <v>234</v>
       </c>
     </row>
@@ -9321,25 +9372,25 @@
       <c r="C36" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="D36" s="29">
+      <c r="D36" s="28">
         <v>25594</v>
       </c>
-      <c r="E36" s="30">
+      <c r="E36" s="29">
         <f t="shared" si="0"/>
         <v>69.928961748633881</v>
       </c>
-      <c r="F36" s="29">
+      <c r="F36" s="28">
         <v>100610</v>
       </c>
-      <c r="G36" s="29" t="s">
+      <c r="G36" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="H36" s="29">
+      <c r="H36" s="28">
         <f>F36*1000</f>
         <v>100610000</v>
       </c>
-      <c r="I36" s="29">
-        <f>H36/D36</f>
+      <c r="I36" s="28">
+        <f t="shared" si="4"/>
         <v>3930.9994529967962</v>
       </c>
     </row>
@@ -9349,27 +9400,27 @@
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="29">
+      <c r="D37" s="28">
         <f>12825000*366/1000000</f>
         <v>4693.95</v>
       </c>
-      <c r="E37" s="30">
+      <c r="E37" s="29">
         <f t="shared" si="0"/>
         <v>12.824999999999999</v>
       </c>
-      <c r="F37" s="29">
+      <c r="F37" s="28">
         <f>130591*366</f>
         <v>47796306</v>
       </c>
-      <c r="G37" s="29" t="s">
+      <c r="G37" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H37" s="29">
+      <c r="H37" s="28">
         <f>F37</f>
         <v>47796306</v>
       </c>
-      <c r="I37" s="29">
-        <f>H37/D37</f>
+      <c r="I37" s="28">
+        <f t="shared" si="4"/>
         <v>10182.534113060428</v>
       </c>
     </row>
@@ -9383,25 +9434,25 @@
       <c r="C38" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="D38" s="29">
+      <c r="D38" s="28">
         <v>9780.0400000000009</v>
       </c>
-      <c r="E38" s="30">
+      <c r="E38" s="29">
         <f t="shared" si="0"/>
         <v>26.721420765027325</v>
       </c>
-      <c r="F38" s="29">
+      <c r="F38" s="28">
         <v>260120703.40000001</v>
       </c>
-      <c r="G38" s="29" t="s">
+      <c r="G38" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H38" s="29">
+      <c r="H38" s="28">
         <f>F38</f>
         <v>260120703.40000001</v>
       </c>
-      <c r="I38" s="29">
-        <f>H38/D38</f>
+      <c r="I38" s="28">
+        <f t="shared" si="4"/>
         <v>26597.10015500959</v>
       </c>
     </row>
@@ -9413,28 +9464,28 @@
       <c r="C39" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D39" s="29">
+      <c r="D39" s="28">
         <v>52532.4</v>
       </c>
-      <c r="E39" s="30">
+      <c r="E39" s="29">
         <f t="shared" si="0"/>
         <v>143.5311475409836</v>
       </c>
-      <c r="F39" s="29">
+      <c r="F39" s="28">
         <v>2000</v>
       </c>
-      <c r="G39" s="29" t="s">
+      <c r="G39" s="28" t="s">
         <v>262</v>
       </c>
-      <c r="H39" s="29">
+      <c r="H39" s="28">
         <f>F39*'Unit conversions'!E3</f>
         <v>1054080000</v>
       </c>
-      <c r="I39" s="29">
-        <f>H39/D39</f>
+      <c r="I39" s="28">
+        <f t="shared" si="4"/>
         <v>20065.331109943578</v>
       </c>
-      <c r="J39" s="29" t="s">
+      <c r="J39" s="28" t="s">
         <v>263</v>
       </c>
     </row>
@@ -9448,25 +9499,25 @@
       <c r="C40" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="D40" s="29">
+      <c r="D40" s="28">
         <v>11125.17</v>
       </c>
-      <c r="E40" s="30">
+      <c r="E40" s="29">
         <f t="shared" si="0"/>
         <v>30.396639344262294</v>
       </c>
-      <c r="F40" s="29">
+      <c r="F40" s="28">
         <v>109251549</v>
       </c>
-      <c r="G40" s="29" t="s">
+      <c r="G40" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H40" s="29">
+      <c r="H40" s="28">
         <f>F40</f>
         <v>109251549</v>
       </c>
-      <c r="I40" s="29">
-        <f>H40/D40</f>
+      <c r="I40" s="28">
+        <f t="shared" si="4"/>
         <v>9820.2138933607312</v>
       </c>
     </row>
@@ -9480,28 +9531,28 @@
       <c r="C41" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="D41" s="29">
+      <c r="D41" s="28">
         <v>53795.15</v>
       </c>
-      <c r="E41" s="30">
+      <c r="E41" s="29">
         <f t="shared" si="0"/>
         <v>146.98128415300548</v>
       </c>
-      <c r="F41" s="29">
+      <c r="F41" s="28">
         <v>230512.4</v>
       </c>
-      <c r="G41" s="29" t="s">
+      <c r="G41" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="H41" s="29">
+      <c r="H41" s="28">
         <f>F41*1000</f>
         <v>230512400</v>
       </c>
-      <c r="I41" s="29">
-        <f>H41/D41</f>
+      <c r="I41" s="28">
+        <f t="shared" si="4"/>
         <v>4285.0033878518789</v>
       </c>
-      <c r="J41" s="29" t="s">
+      <c r="J41" s="28" t="s">
         <v>88</v>
       </c>
     </row>
@@ -9515,28 +9566,28 @@
       <c r="C42" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="D42" s="29">
+      <c r="D42" s="28">
         <v>39234.039989999997</v>
       </c>
-      <c r="E42" s="30">
+      <c r="E42" s="29">
         <f t="shared" si="0"/>
         <v>107.19683057377048</v>
       </c>
-      <c r="F42" s="29">
+      <c r="F42" s="28">
         <v>3091256</v>
       </c>
-      <c r="G42" s="29" t="s">
+      <c r="G42" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="H42" s="29">
+      <c r="H42" s="28">
         <f>F42*'Unit conversions'!E2</f>
         <v>515209333.33333337</v>
       </c>
-      <c r="I42" s="29">
-        <f>H42/D42</f>
+      <c r="I42" s="28">
+        <f t="shared" si="4"/>
         <v>13131.69210880782</v>
       </c>
-      <c r="J42" s="29">
+      <c r="J42" s="28">
         <v>37014310</v>
       </c>
     </row>
@@ -9550,25 +9601,25 @@
       <c r="C43" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="D43" s="29">
+      <c r="D43" s="28">
         <v>2114.1046000000001</v>
       </c>
-      <c r="E43" s="30">
+      <c r="E43" s="29">
         <f t="shared" si="0"/>
         <v>5.7762420765027329</v>
       </c>
-      <c r="F43" s="29">
+      <c r="F43" s="28">
         <v>22684790</v>
       </c>
-      <c r="G43" s="29" t="s">
+      <c r="G43" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H43" s="29">
+      <c r="H43" s="28">
         <f>F43</f>
         <v>22684790</v>
       </c>
-      <c r="I43" s="29">
-        <f>H43/D43</f>
+      <c r="I43" s="28">
+        <f t="shared" si="4"/>
         <v>10730.211740705734</v>
       </c>
     </row>
@@ -9582,26 +9633,26 @@
       <c r="C44" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="D44" s="29">
+      <c r="D44" s="28">
         <f>37403.85</f>
         <v>37403.85</v>
       </c>
-      <c r="E44" s="30">
+      <c r="E44" s="29">
         <f t="shared" si="0"/>
         <v>102.19631147540983</v>
       </c>
-      <c r="F44" s="29">
+      <c r="F44" s="28">
         <v>525983532</v>
       </c>
-      <c r="G44" s="29" t="s">
+      <c r="G44" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H44" s="29">
+      <c r="H44" s="28">
         <f>F44</f>
         <v>525983532</v>
       </c>
-      <c r="I44" s="29">
-        <f>H44/D44</f>
+      <c r="I44" s="28">
+        <f t="shared" si="4"/>
         <v>14062.283214161109</v>
       </c>
     </row>
@@ -9615,25 +9666,25 @@
       <c r="C45" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="D45" s="29">
+      <c r="D45" s="28">
         <v>12352.05</v>
       </c>
-      <c r="E45" s="30">
+      <c r="E45" s="29">
         <f t="shared" si="0"/>
         <v>33.748770491803278</v>
       </c>
-      <c r="F45" s="29">
+      <c r="F45" s="28">
         <v>1377065.72</v>
       </c>
-      <c r="G45" s="29" t="s">
+      <c r="G45" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="H45" s="29">
+      <c r="H45" s="28">
         <f>F45*'Unit conversions'!E2</f>
         <v>229510953.33333334</v>
       </c>
-      <c r="I45" s="29">
-        <f>H45/D45</f>
+      <c r="I45" s="28">
+        <f t="shared" si="4"/>
         <v>18580.798598883048</v>
       </c>
     </row>
@@ -9647,25 +9698,25 @@
       <c r="C46" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="D46" s="29">
+      <c r="D46" s="28">
         <v>20935.599999999999</v>
       </c>
-      <c r="E46" s="30">
+      <c r="E46" s="29">
         <f t="shared" si="0"/>
         <v>57.201092896174856</v>
       </c>
-      <c r="F46" s="29">
+      <c r="F46" s="28">
         <v>198866597</v>
       </c>
-      <c r="G46" s="29" t="s">
+      <c r="G46" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H46" s="29">
+      <c r="H46" s="28">
         <f>F46</f>
         <v>198866597</v>
       </c>
-      <c r="I46" s="29">
-        <f>H46/D46</f>
+      <c r="I46" s="28">
+        <f t="shared" si="4"/>
         <v>9498.9681212862306</v>
       </c>
     </row>
@@ -9679,26 +9730,26 @@
       <c r="C47" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="D47" s="29">
+      <c r="D47" s="28">
         <v>864.41</v>
       </c>
-      <c r="E47" s="30">
+      <c r="E47" s="29">
         <f t="shared" si="0"/>
         <v>2.3617759562841529</v>
       </c>
-      <c r="F47" s="29">
+      <c r="F47" s="28">
         <f>1022504*12</f>
         <v>12270048</v>
       </c>
-      <c r="G47" s="29" t="s">
+      <c r="G47" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H47" s="29">
+      <c r="H47" s="28">
         <f>F47</f>
         <v>12270048</v>
       </c>
-      <c r="I47" s="29">
-        <f>H47/D47</f>
+      <c r="I47" s="28">
+        <f t="shared" si="4"/>
         <v>14194.708529517244</v>
       </c>
       <c r="K47" s="4" t="s">
@@ -9715,67 +9766,67 @@
       <c r="C48" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="D48" s="29">
+      <c r="D48" s="28">
         <v>21818</v>
       </c>
-      <c r="E48" s="30">
+      <c r="E48" s="29">
         <f t="shared" si="0"/>
         <v>59.612021857923494</v>
       </c>
-      <c r="F48" s="29">
+      <c r="F48" s="28">
         <v>222437605</v>
       </c>
-      <c r="G48" s="29" t="s">
+      <c r="G48" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H48" s="29">
+      <c r="H48" s="28">
         <f>F48</f>
         <v>222437605</v>
       </c>
-      <c r="I48" s="29">
-        <f>H48/D48</f>
+      <c r="I48" s="28">
+        <f t="shared" si="4"/>
         <v>10195.141855348795</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="24" t="s">
+    <row r="49" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="B49" s="25" t="s">
+      <c r="B49" s="24" t="s">
         <v>324</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="24" t="s">
         <v>325</v>
       </c>
-      <c r="D49" s="28">
+      <c r="D49" s="27">
         <v>1247.2</v>
       </c>
-      <c r="E49" s="31">
+      <c r="E49" s="30">
         <f t="shared" si="0"/>
         <v>3.4076502732240437</v>
       </c>
-      <c r="F49" s="28">
+      <c r="F49" s="27">
         <f>200000*366</f>
         <v>73200000</v>
       </c>
-      <c r="G49" s="28" t="s">
+      <c r="G49" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="H49" s="28">
+      <c r="H49" s="27">
         <f>F49</f>
         <v>73200000</v>
       </c>
-      <c r="I49" s="28">
-        <f>H49/D49</f>
+      <c r="I49" s="27">
+        <f t="shared" si="4"/>
         <v>58691.468890314303</v>
       </c>
-      <c r="J49" s="28">
+      <c r="J49" s="27">
         <v>1013708.59</v>
       </c>
-      <c r="K49" s="26" t="s">
+      <c r="K49" s="25" t="s">
         <v>327</v>
       </c>
     </row>
@@ -9789,28 +9840,28 @@
       <c r="C50" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="D50" s="29">
+      <c r="D50" s="28">
         <v>8220.6</v>
       </c>
-      <c r="E50" s="30">
+      <c r="E50" s="29">
         <f t="shared" si="0"/>
         <v>22.460655737704919</v>
       </c>
-      <c r="F50" s="29">
+      <c r="F50" s="28">
         <v>45950</v>
       </c>
-      <c r="G50" s="29" t="s">
+      <c r="G50" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="H50" s="29">
+      <c r="H50" s="28">
         <f>F50*'Unit conversions'!E4</f>
         <v>76583333.333333343</v>
       </c>
-      <c r="I50" s="29">
-        <f>H50/D50</f>
+      <c r="I50" s="28">
+        <f t="shared" si="4"/>
         <v>9316.0272161804896</v>
       </c>
-      <c r="J50" s="29"/>
+      <c r="J50" s="28"/>
       <c r="K50" s="3" t="s">
         <v>333</v>
       </c>
@@ -9825,31 +9876,1004 @@
       <c r="C51" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="D51" s="29">
+      <c r="D51" s="28">
         <v>12110.7</v>
       </c>
-      <c r="E51" s="30">
+      <c r="E51" s="29">
         <f t="shared" si="0"/>
         <v>33.089344262295086</v>
       </c>
-      <c r="F51" s="44">
+      <c r="F51" s="40">
         <f>SUM(A51:D51)</f>
         <v>12110.7</v>
       </c>
-      <c r="G51" s="29" t="s">
+      <c r="G51" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="H51" s="29">
+      <c r="H51" s="28">
         <f>F51*'Unit conversions'!E4</f>
         <v>20184500.000000004</v>
       </c>
-      <c r="I51" s="29">
-        <f>H51/D51</f>
+      <c r="I51" s="28">
+        <f t="shared" si="4"/>
         <v>1666.666666666667</v>
       </c>
-      <c r="J51" s="29"/>
+      <c r="J51" s="28"/>
       <c r="K51" s="3" t="s">
         <v>333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B50971E-30C9-3346-9F59-C7F18C75FF5F}">
+  <dimension ref="A1:F48"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.2">
+      <c r="A1" s="41" t="s">
+        <v>359</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>399</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>400</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="44">
+        <v>12180.39</v>
+      </c>
+      <c r="E2" s="44">
+        <v>33.28</v>
+      </c>
+      <c r="F2" s="44">
+        <v>137991.38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="44">
+        <v>4989.95</v>
+      </c>
+      <c r="E3" s="44">
+        <v>13.63</v>
+      </c>
+      <c r="F3" s="44">
+        <v>59659000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A4" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="48">
+        <v>48275.4</v>
+      </c>
+      <c r="E4" s="48">
+        <v>131.9</v>
+      </c>
+      <c r="F4" s="48">
+        <v>4021242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="44">
+        <v>5515.83</v>
+      </c>
+      <c r="E5" s="44">
+        <v>15.07</v>
+      </c>
+      <c r="F5" s="44">
+        <v>86030950</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="44">
+        <v>4564.37</v>
+      </c>
+      <c r="E6" s="44">
+        <v>12.47</v>
+      </c>
+      <c r="F6" s="44">
+        <v>49347000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="44">
+        <v>41314</v>
+      </c>
+      <c r="E7" s="44">
+        <v>112.88</v>
+      </c>
+      <c r="F7" s="44">
+        <v>174134200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="49">
+        <v>2921.9</v>
+      </c>
+      <c r="E8" s="44">
+        <v>7.98</v>
+      </c>
+      <c r="F8" s="44">
+        <v>111328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="49">
+        <v>8681.7999999999993</v>
+      </c>
+      <c r="E9" s="44">
+        <v>23.72</v>
+      </c>
+      <c r="F9" s="44">
+        <v>457588</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="49">
+        <v>224980</v>
+      </c>
+      <c r="E10" s="44">
+        <v>614.70000000000005</v>
+      </c>
+      <c r="F10" s="44">
+        <v>1093162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A11" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="48">
+        <v>45980.6</v>
+      </c>
+      <c r="E11" s="48">
+        <v>125.63</v>
+      </c>
+      <c r="F11" s="48">
+        <v>968752.82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="105" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="44">
+        <v>13070.65</v>
+      </c>
+      <c r="E12" s="44">
+        <v>35.71</v>
+      </c>
+      <c r="F12" s="44">
+        <v>206329392</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="44">
+        <v>10486.9</v>
+      </c>
+      <c r="E13" s="44">
+        <v>28.65</v>
+      </c>
+      <c r="F13" s="44">
+        <v>121391220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="44">
+        <v>6945.31</v>
+      </c>
+      <c r="E14" s="44">
+        <v>18.98</v>
+      </c>
+      <c r="F14" s="44">
+        <v>78667674</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="44">
+        <v>2321.3200000000002</v>
+      </c>
+      <c r="E15" s="44">
+        <v>6.34</v>
+      </c>
+      <c r="F15" s="44">
+        <v>29680770</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="44">
+        <v>15202.37</v>
+      </c>
+      <c r="E16" s="44">
+        <v>41.54</v>
+      </c>
+      <c r="F16" s="44">
+        <v>159260997.59999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="44">
+        <v>4388.58</v>
+      </c>
+      <c r="E17" s="44">
+        <v>11.99</v>
+      </c>
+      <c r="F17" s="44">
+        <v>51331878</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" s="44">
+        <v>17185.400000000001</v>
+      </c>
+      <c r="E18" s="44">
+        <v>46.95</v>
+      </c>
+      <c r="F18" s="44">
+        <v>284977.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D19" s="44">
+        <v>549.65</v>
+      </c>
+      <c r="E19" s="44">
+        <v>1.5</v>
+      </c>
+      <c r="F19" s="44">
+        <v>3709528</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D20" s="44">
+        <v>1374.44</v>
+      </c>
+      <c r="E20" s="44">
+        <v>3.76</v>
+      </c>
+      <c r="F20" s="44">
+        <v>22284115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" s="44">
+        <v>1932.74</v>
+      </c>
+      <c r="E21" s="44">
+        <v>5.28</v>
+      </c>
+      <c r="F21" s="44">
+        <v>38351800</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="D22" s="44">
+        <v>14426.1</v>
+      </c>
+      <c r="E22" s="44">
+        <v>39.42</v>
+      </c>
+      <c r="F22" s="44">
+        <v>236718970</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="D23" s="44">
+        <v>8699.59</v>
+      </c>
+      <c r="E23" s="44">
+        <v>23.77</v>
+      </c>
+      <c r="F23" s="44">
+        <v>133967709.40000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="D24" s="44">
+        <v>823.03</v>
+      </c>
+      <c r="E24" s="44">
+        <v>2.25</v>
+      </c>
+      <c r="F24" s="44">
+        <v>6468208.7000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A25" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="D25" s="44">
+        <v>38173.980000000003</v>
+      </c>
+      <c r="E25" s="44">
+        <v>104.3</v>
+      </c>
+      <c r="F25" s="44">
+        <v>415332388.10000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A26" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="D26" s="44">
+        <v>13410.74</v>
+      </c>
+      <c r="E26" s="44">
+        <v>36.64</v>
+      </c>
+      <c r="F26" s="44">
+        <v>331468584.19999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A27" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="D27" s="44">
+        <v>13420</v>
+      </c>
+      <c r="E27" s="44">
+        <v>36.67</v>
+      </c>
+      <c r="F27" s="44">
+        <v>331.36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A28" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="D28" s="44">
+        <v>29126.9</v>
+      </c>
+      <c r="E28" s="44">
+        <v>79.58</v>
+      </c>
+      <c r="F28" s="44">
+        <v>338700000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A29" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" s="47" t="s">
+        <v>197</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="D29" s="48">
+        <v>24848.799999999999</v>
+      </c>
+      <c r="E29" s="48">
+        <v>67.89</v>
+      </c>
+      <c r="F29" s="48">
+        <v>1085100000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A30" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="D30" s="48">
+        <v>57285</v>
+      </c>
+      <c r="E30" s="48">
+        <v>156.52000000000001</v>
+      </c>
+      <c r="F30" s="48">
+        <v>128009</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A31" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="D31" s="44">
+        <v>25594</v>
+      </c>
+      <c r="E31" s="44">
+        <v>69.930000000000007</v>
+      </c>
+      <c r="F31" s="44">
+        <v>1072223</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A32" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="D32" s="44">
+        <v>29658.69</v>
+      </c>
+      <c r="E32" s="44">
+        <v>81.03</v>
+      </c>
+      <c r="F32" s="51">
+        <v>132.88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A33" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="D33" s="44">
+        <v>25594</v>
+      </c>
+      <c r="E33" s="44">
+        <v>69.930000000000007</v>
+      </c>
+      <c r="F33" s="44">
+        <v>100610</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="44">
+        <v>4693.95</v>
+      </c>
+      <c r="E34" s="44">
+        <v>12.83</v>
+      </c>
+      <c r="F34" s="44">
+        <v>47796306</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A35" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="D35" s="44">
+        <v>9780.0400000000009</v>
+      </c>
+      <c r="E35" s="44">
+        <v>26.72</v>
+      </c>
+      <c r="F35" s="44">
+        <v>260120703.40000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A36" s="20" t="s">
+        <v>259</v>
+      </c>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="D36" s="44">
+        <v>52532.4</v>
+      </c>
+      <c r="E36" s="44">
+        <v>143.53</v>
+      </c>
+      <c r="F36" s="44">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A37" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="D37" s="44">
+        <v>11125.17</v>
+      </c>
+      <c r="E37" s="44">
+        <v>30.4</v>
+      </c>
+      <c r="F37" s="44">
+        <v>109251549</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A38" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="D38" s="44">
+        <v>53795.15</v>
+      </c>
+      <c r="E38" s="44">
+        <v>146.97999999999999</v>
+      </c>
+      <c r="F38" s="44">
+        <v>230512.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A39" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="D39" s="44">
+        <v>39234.04</v>
+      </c>
+      <c r="E39" s="44">
+        <v>107.2</v>
+      </c>
+      <c r="F39" s="44">
+        <v>3091256</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="D40" s="44">
+        <v>2114.1</v>
+      </c>
+      <c r="E40" s="44">
+        <v>5.78</v>
+      </c>
+      <c r="F40" s="44">
+        <v>22684790</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A41" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="D41" s="44">
+        <v>37403.85</v>
+      </c>
+      <c r="E41" s="44">
+        <v>102.2</v>
+      </c>
+      <c r="F41" s="44">
+        <v>525983532</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A42" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="D42" s="44">
+        <v>12352.05</v>
+      </c>
+      <c r="E42" s="44">
+        <v>33.75</v>
+      </c>
+      <c r="F42" s="44">
+        <v>1377065.72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A43" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="D43" s="44">
+        <v>20935.599999999999</v>
+      </c>
+      <c r="E43" s="44">
+        <v>57.2</v>
+      </c>
+      <c r="F43" s="44">
+        <v>198866597</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A44" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="D44" s="44">
+        <v>864.41</v>
+      </c>
+      <c r="E44" s="44">
+        <v>2.36</v>
+      </c>
+      <c r="F44" s="44">
+        <v>12270048</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="120" x14ac:dyDescent="0.2">
+      <c r="A45" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="D45" s="44">
+        <v>21818</v>
+      </c>
+      <c r="E45" s="44">
+        <v>59.61</v>
+      </c>
+      <c r="F45" s="44">
+        <v>222437605</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A46" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="B46" s="47" t="s">
+        <v>324</v>
+      </c>
+      <c r="C46" s="47" t="s">
+        <v>325</v>
+      </c>
+      <c r="D46" s="48">
+        <v>1247.2</v>
+      </c>
+      <c r="E46" s="48">
+        <v>3.41</v>
+      </c>
+      <c r="F46" s="48">
+        <v>73200000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A47" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="D47" s="44">
+        <v>8220.6</v>
+      </c>
+      <c r="E47" s="44">
+        <v>22.46</v>
+      </c>
+      <c r="F47" s="44">
+        <v>45950</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A48" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="D48" s="44">
+        <v>12110.7</v>
+      </c>
+      <c r="E48" s="44">
+        <v>33.090000000000003</v>
+      </c>
+      <c r="F48" s="51">
+        <v>12110.7</v>
       </c>
     </row>
   </sheetData>
@@ -9857,7 +10881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A7E812-EA3F-DD4E-B968-0754A5398D5F}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -9874,23 +10898,23 @@
       <c r="A1" s="21" t="s">
         <v>359</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>360</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>361</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" t="s">
         <v>369</v>
       </c>
     </row>
@@ -9898,7 +10922,7 @@
       <c r="A4" s="21" t="s">
         <v>362</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" t="s">
         <v>370</v>
       </c>
     </row>
@@ -9906,7 +10930,7 @@
       <c r="A5" s="21" t="s">
         <v>363</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" t="s">
         <v>371</v>
       </c>
     </row>
@@ -9914,7 +10938,7 @@
       <c r="A6" s="21" t="s">
         <v>364</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" t="s">
         <v>372</v>
       </c>
     </row>
@@ -9922,7 +10946,7 @@
       <c r="A7" s="21" t="s">
         <v>366</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" t="s">
         <v>373</v>
       </c>
     </row>
@@ -9930,7 +10954,7 @@
       <c r="A8" s="21" t="s">
         <v>365</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" t="s">
         <v>374</v>
       </c>
     </row>
@@ -9938,7 +10962,7 @@
       <c r="A9" s="21" t="s">
         <v>376</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" t="s">
         <v>375</v>
       </c>
     </row>
@@ -9946,7 +10970,7 @@
       <c r="A10" s="21" t="s">
         <v>377</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" t="s">
         <v>378</v>
       </c>
     </row>
@@ -9955,12 +10979,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B12C50-DC4E-5D46-A39D-190792E41EE6}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10054,7 +11078,7 @@
         <v>397</v>
       </c>
       <c r="C4">
-        <f>A2*K3*(1/K2)*(1/K4)</f>
+        <f>A4*K3*(1/K2)*(1/K4)</f>
         <v>1666.666666666667</v>
       </c>
       <c r="D4" t="s">
@@ -10076,49 +11100,49 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8BE7CE-B762-A34D-B973-D222CD1757B8}">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" style="39" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" style="39" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" style="35" customWidth="1"/>
     <col min="17" max="17" width="16.1640625" customWidth="1"/>
-    <col min="18" max="18" width="24.1640625" style="39" customWidth="1"/>
-    <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.83203125" style="39" customWidth="1"/>
+    <col min="18" max="18" width="24.1640625" style="35" customWidth="1"/>
+    <col min="19" max="19" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.83203125" style="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>359</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="32" t="s">
         <v>391</v>
       </c>
       <c r="C1" t="s">
         <v>366</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="32" t="s">
         <v>380</v>
       </c>
       <c r="Q1" s="13" t="s">
         <v>359</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="32" t="s">
         <v>391</v>
       </c>
       <c r="S1" t="s">
         <v>366</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="32" t="s">
         <v>380</v>
       </c>
     </row>
@@ -10126,43 +11150,43 @@
       <c r="A2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="29">
         <v>56.436311475409831</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="30"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="29"/>
       <c r="Q2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="30">
+      <c r="R2" s="29">
         <v>56.436311475409831</v>
       </c>
-      <c r="S2" s="39"/>
-      <c r="T2" s="30"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="29"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="29">
         <v>33.279748633879784</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="35">
         <v>137991378.20000002</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>11328.980505382917</v>
       </c>
       <c r="Q3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="R3" s="30">
+      <c r="R3" s="29">
         <v>33.279748633879784</v>
       </c>
-      <c r="S3" s="39">
+      <c r="S3" s="35">
         <v>137991378.20000002</v>
       </c>
-      <c r="T3" s="30">
+      <c r="T3" s="29">
         <v>11328.980505382917</v>
       </c>
     </row>
@@ -10170,47 +11194,47 @@
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="29">
         <v>13.633737704918033</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="35">
         <v>59659000</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="29">
         <v>11955.836012719972</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="R4" s="30">
+      <c r="R4" s="29">
         <v>13.633737704918033</v>
       </c>
-      <c r="S4" s="39">
+      <c r="S4" s="35">
         <v>59659000</v>
       </c>
-      <c r="T4" s="30">
+      <c r="T4" s="29">
         <v>11955.836012719972</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="30">
         <v>131.9</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="35">
         <v>4021242000</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="30">
         <v>83297.95299469294</v>
       </c>
-      <c r="Q5" s="24" t="s">
+      <c r="Q5" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="R5" s="31"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="31">
+      <c r="R5" s="30"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="30">
         <v>83297.95299469294</v>
       </c>
     </row>
@@ -10218,25 +11242,25 @@
       <c r="A6" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="29">
         <v>15.070573770491803</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="35">
         <v>86030950</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="29">
         <v>15597.099620546682</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="R6" s="30">
+      <c r="R6" s="29">
         <v>15.070573770491803</v>
       </c>
-      <c r="S6" s="39">
+      <c r="S6" s="35">
         <v>86030950</v>
       </c>
-      <c r="T6" s="30">
+      <c r="T6" s="29">
         <v>15597.099620546682</v>
       </c>
     </row>
@@ -10244,25 +11268,25 @@
       <c r="A7" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="29">
         <v>12.470956284153004</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="35">
         <v>49347000</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="29">
         <v>10811.349649568287</v>
       </c>
       <c r="Q7" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="R7" s="30">
+      <c r="R7" s="29">
         <v>12.470956284153004</v>
       </c>
-      <c r="S7" s="39">
+      <c r="S7" s="35">
         <v>49347000</v>
       </c>
-      <c r="T7" s="30">
+      <c r="T7" s="29">
         <v>10811.349649568287</v>
       </c>
     </row>
@@ -10270,25 +11294,25 @@
       <c r="A8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="29">
         <v>112.87978142076503</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C8" s="35">
         <v>174134200</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="29">
         <v>4214.8956770102141</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="R8" s="30">
+      <c r="R8" s="29">
         <v>112.87978142076503</v>
       </c>
-      <c r="S8" s="39">
+      <c r="S8" s="35">
         <v>174134200</v>
       </c>
-      <c r="T8" s="30">
+      <c r="T8" s="29">
         <v>4214.8956770102141</v>
       </c>
     </row>
@@ -10296,25 +11320,25 @@
       <c r="A9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="29">
         <v>7.9833333333333334</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="35">
         <v>18554666.666666668</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="28">
         <v>6350.2059162417154</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="R9" s="30">
+      <c r="R9" s="29">
         <v>7.9833333333333334</v>
       </c>
-      <c r="S9" s="39">
+      <c r="S9" s="35">
         <v>18554666.666666668</v>
       </c>
-      <c r="T9" s="29">
+      <c r="T9" s="28">
         <v>6350.2059162417154</v>
       </c>
     </row>
@@ -10322,73 +11346,73 @@
       <c r="A10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="29">
         <v>23.720765027322404</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="35">
         <v>76264666.666666672</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="28">
         <v>8784.430264077344</v>
       </c>
       <c r="Q10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="R10" s="30">
+      <c r="R10" s="29">
         <v>23.720765027322404</v>
       </c>
-      <c r="S10" s="39">
+      <c r="S10" s="35">
         <v>76264666.666666672</v>
       </c>
-      <c r="T10" s="29">
+      <c r="T10" s="28">
         <v>8784.430264077344</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="B11" s="42">
+      <c r="B11" s="30">
         <v>614.6994535519126</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="34">
         <v>182193666.66666669</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="27">
         <v>809.82161377307625</v>
       </c>
-      <c r="Q11" s="32" t="s">
+      <c r="Q11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="R11" s="42"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="34">
+      <c r="R11" s="38"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="31">
         <v>809.82161377307625</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="30">
         <v>125.63005867459017</v>
       </c>
-      <c r="C12" s="39">
+      <c r="C12" s="35">
         <v>968752819.45899999</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="27">
         <v>21068.728733090302</v>
       </c>
-      <c r="Q12" s="24" t="s">
+      <c r="Q12" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="R12" s="31">
+      <c r="R12" s="30">
         <v>125.63005867459017</v>
       </c>
-      <c r="S12" s="39">
+      <c r="S12" s="35">
         <v>968752819.45899999</v>
       </c>
-      <c r="T12" s="28">
+      <c r="T12" s="27">
         <v>21068.728733090302</v>
       </c>
     </row>
@@ -10396,25 +11420,25 @@
       <c r="A13" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="29">
         <v>35.712158469945351</v>
       </c>
-      <c r="C13" s="39">
+      <c r="C13" s="35">
         <v>206329392</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="28">
         <v>15785.702470802906</v>
       </c>
       <c r="Q13" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="R13" s="30">
+      <c r="R13" s="29">
         <v>35.712158469945351</v>
       </c>
-      <c r="S13" s="39">
+      <c r="S13" s="35">
         <v>206329392</v>
       </c>
-      <c r="T13" s="29">
+      <c r="T13" s="28">
         <v>15785.702470802906</v>
       </c>
     </row>
@@ -10422,25 +11446,25 @@
       <c r="A14" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="29">
         <v>28.652732240437157</v>
       </c>
-      <c r="C14" s="39">
+      <c r="C14" s="35">
         <v>121391220</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="28">
         <v>11575.510398687888</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="R14" s="30">
+      <c r="R14" s="29">
         <v>28.652732240437157</v>
       </c>
-      <c r="S14" s="39">
+      <c r="S14" s="35">
         <v>121391220</v>
       </c>
-      <c r="T14" s="29">
+      <c r="T14" s="28">
         <v>11575.510398687888</v>
       </c>
     </row>
@@ -10448,25 +11472,25 @@
       <c r="A15" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="30">
+      <c r="B15" s="29">
         <v>18.976256830601095</v>
       </c>
-      <c r="C15" s="39">
+      <c r="C15" s="35">
         <v>78667674</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="28">
         <v>11326.73329196249</v>
       </c>
       <c r="Q15" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="R15" s="30">
+      <c r="R15" s="29">
         <v>18.976256830601095</v>
       </c>
-      <c r="S15" s="39">
+      <c r="S15" s="35">
         <v>78667674</v>
       </c>
-      <c r="T15" s="29">
+      <c r="T15" s="28">
         <v>11326.73329196249</v>
       </c>
     </row>
@@ -10474,25 +11498,25 @@
       <c r="A16" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="29">
         <v>6.3424043715847001</v>
       </c>
-      <c r="C16" s="39">
+      <c r="C16" s="35">
         <v>29680770</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="28">
         <v>12786.160460427687</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="R16" s="30">
+      <c r="R16" s="29">
         <v>6.3424043715847001</v>
       </c>
-      <c r="S16" s="39">
+      <c r="S16" s="35">
         <v>29680770</v>
       </c>
-      <c r="T16" s="29">
+      <c r="T16" s="28">
         <v>12786.160460427687</v>
       </c>
     </row>
@@ -10500,25 +11524,25 @@
       <c r="A17" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B17" s="29">
         <v>41.536532704918031</v>
       </c>
-      <c r="C17" s="39">
+      <c r="C17" s="35">
         <v>159260997.59999999</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="28">
         <v>10476.063103201592</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="R17" s="30">
+      <c r="R17" s="29">
         <v>41.536532704918031</v>
       </c>
-      <c r="S17" s="39">
+      <c r="S17" s="35">
         <v>159260997.59999999</v>
       </c>
-      <c r="T17" s="29">
+      <c r="T17" s="28">
         <v>10476.063103201592</v>
       </c>
     </row>
@@ -10526,25 +11550,25 @@
       <c r="A18" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B18" s="29">
         <v>11.990642076502732</v>
       </c>
-      <c r="C18" s="39">
+      <c r="C18" s="35">
         <v>51331878</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="28">
         <v>11696.70747338259</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="R18" s="30">
+      <c r="R18" s="29">
         <v>11.990642076502732</v>
       </c>
-      <c r="S18" s="39">
+      <c r="S18" s="35">
         <v>51331878</v>
       </c>
-      <c r="T18" s="29">
+      <c r="T18" s="28">
         <v>11696.70747338259</v>
       </c>
     </row>
@@ -10552,25 +11576,25 @@
       <c r="A19" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="29">
         <v>46.954644808743176</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="35">
         <v>284977500</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="28">
         <v>16582.53517520686</v>
       </c>
       <c r="Q19" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="R19" s="30">
+      <c r="R19" s="29">
         <v>46.954644808743176</v>
       </c>
-      <c r="S19" s="39">
+      <c r="S19" s="35">
         <v>284977500</v>
       </c>
-      <c r="T19" s="29">
+      <c r="T19" s="28">
         <v>16582.53517520686</v>
       </c>
     </row>
@@ -10578,25 +11602,25 @@
       <c r="A20" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B20" s="30">
+      <c r="B20" s="29">
         <v>1.5017759562841528</v>
       </c>
-      <c r="C20" s="39">
+      <c r="C20" s="35">
         <v>3709528</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="28">
         <v>6748.8911125261529</v>
       </c>
       <c r="Q20" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="R20" s="30">
+      <c r="R20" s="29">
         <v>1.5017759562841528</v>
       </c>
-      <c r="S20" s="39">
+      <c r="S20" s="35">
         <v>3709528</v>
       </c>
-      <c r="T20" s="29">
+      <c r="T20" s="28">
         <v>6748.8911125261529</v>
       </c>
     </row>
@@ -10604,25 +11628,25 @@
       <c r="A21" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B21" s="30">
+      <c r="B21" s="29">
         <v>3.7553005464480878</v>
       </c>
-      <c r="C21" s="39">
+      <c r="C21" s="35">
         <v>22284115</v>
       </c>
-      <c r="D21" s="29">
+      <c r="D21" s="28">
         <v>16213.232298245102</v>
       </c>
       <c r="Q21" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="R21" s="30">
+      <c r="R21" s="29">
         <v>3.7553005464480878</v>
       </c>
-      <c r="S21" s="39">
+      <c r="S21" s="35">
         <v>22284115</v>
       </c>
-      <c r="T21" s="29">
+      <c r="T21" s="28">
         <v>16213.232298245102</v>
       </c>
     </row>
@@ -10630,61 +11654,61 @@
       <c r="A22" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B22" s="29">
         <v>5.2807103825136616</v>
       </c>
-      <c r="C22" s="39">
+      <c r="C22" s="35">
         <v>38351800</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="28">
         <v>19843.227749205791</v>
       </c>
       <c r="Q22" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="R22" s="30">
+      <c r="R22" s="29">
         <v>5.2807103825136616</v>
       </c>
-      <c r="S22" s="39">
+      <c r="S22" s="35">
         <v>38351800</v>
       </c>
-      <c r="T22" s="29">
+      <c r="T22" s="28">
         <v>19843.227749205791</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="28"/>
       <c r="Q23" s="2"/>
-      <c r="R23" s="30"/>
-      <c r="S23" s="39"/>
-      <c r="T23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="35"/>
+      <c r="T23" s="28"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B24" s="30">
+      <c r="B24" s="29">
         <v>39.415573770491804</v>
       </c>
-      <c r="C24" s="39">
+      <c r="C24" s="35">
         <v>236718970</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="28">
         <v>16409.075911022384</v>
       </c>
       <c r="Q24" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="R24" s="30">
+      <c r="R24" s="29">
         <v>39.415573770491804</v>
       </c>
-      <c r="S24" s="39">
+      <c r="S24" s="35">
         <v>236718970</v>
       </c>
-      <c r="T24" s="29">
+      <c r="T24" s="28">
         <v>16409.075911022384</v>
       </c>
     </row>
@@ -10692,25 +11716,25 @@
       <c r="A25" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B25" s="30">
+      <c r="B25" s="29">
         <v>23.76937081967213</v>
       </c>
-      <c r="C25" s="39">
+      <c r="C25" s="35">
         <v>133967709.40000001</v>
       </c>
-      <c r="D25" s="29">
+      <c r="D25" s="28">
         <v>15399.313497740444</v>
       </c>
       <c r="Q25" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="R25" s="30">
+      <c r="R25" s="29">
         <v>23.76937081967213</v>
       </c>
-      <c r="S25" s="39">
+      <c r="S25" s="35">
         <v>133967709.40000001</v>
       </c>
-      <c r="T25" s="29">
+      <c r="T25" s="28">
         <v>15399.313497740444</v>
       </c>
     </row>
@@ -10718,25 +11742,25 @@
       <c r="A26" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B26" s="30">
+      <c r="B26" s="29">
         <v>2.248712382513661</v>
       </c>
-      <c r="C26" s="39">
+      <c r="C26" s="35">
         <v>6468208.7000000002</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="28">
         <v>7859.0314633146982</v>
       </c>
       <c r="Q26" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="R26" s="30">
+      <c r="R26" s="29">
         <v>2.248712382513661</v>
       </c>
-      <c r="S26" s="39">
+      <c r="S26" s="35">
         <v>6468208.7000000002</v>
       </c>
-      <c r="T26" s="29">
+      <c r="T26" s="28">
         <v>7859.0314633146982</v>
       </c>
     </row>
@@ -10744,25 +11768,25 @@
       <c r="A27" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B27" s="30">
+      <c r="B27" s="29">
         <v>104.3004918032787</v>
       </c>
-      <c r="C27" s="39">
+      <c r="C27" s="35">
         <v>415332388.10000002</v>
       </c>
-      <c r="D27" s="29">
+      <c r="D27" s="28">
         <v>10879.986527472378</v>
       </c>
       <c r="Q27" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="R27" s="30">
+      <c r="R27" s="29">
         <v>104.3004918032787</v>
       </c>
-      <c r="S27" s="39">
+      <c r="S27" s="35">
         <v>415332388.10000002</v>
       </c>
-      <c r="T27" s="29">
+      <c r="T27" s="28">
         <v>10879.986527472378</v>
       </c>
     </row>
@@ -10770,25 +11794,25 @@
       <c r="A28" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B28" s="30">
+      <c r="B28" s="29">
         <v>36.641374316939888</v>
       </c>
-      <c r="C28" s="39">
+      <c r="C28" s="35">
         <v>331468584.19999999</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="28">
         <v>24716.645766755799</v>
       </c>
       <c r="Q28" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="R28" s="30">
+      <c r="R28" s="29">
         <v>36.641374316939888</v>
       </c>
-      <c r="S28" s="39">
+      <c r="S28" s="35">
         <v>331468584.19999999</v>
       </c>
-      <c r="T28" s="29">
+      <c r="T28" s="28">
         <v>24716.645766755799</v>
       </c>
     </row>
@@ -10796,25 +11820,25 @@
       <c r="A29" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="B29" s="30">
+      <c r="B29" s="29">
         <v>36.666666666666664</v>
       </c>
-      <c r="C29" s="39">
+      <c r="C29" s="35">
         <v>331360000</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="28">
         <v>24691.505216095378</v>
       </c>
       <c r="Q29" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="R29" s="30">
+      <c r="R29" s="29">
         <v>36.666666666666664</v>
       </c>
-      <c r="S29" s="39">
+      <c r="S29" s="35">
         <v>331360000</v>
       </c>
-      <c r="T29" s="29">
+      <c r="T29" s="28">
         <v>24691.505216095378</v>
       </c>
     </row>
@@ -10822,101 +11846,105 @@
       <c r="A30" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B30" s="30">
+      <c r="B30" s="29">
         <v>79.581693989071042</v>
       </c>
-      <c r="C30" s="39">
+      <c r="C30" s="35">
         <v>338700000</v>
       </c>
-      <c r="D30" s="29">
+      <c r="D30" s="28">
         <v>11628.425956761619</v>
       </c>
       <c r="Q30" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="R30" s="30">
+      <c r="R30" s="29">
         <v>79.581693989071042</v>
       </c>
-      <c r="S30" s="39">
+      <c r="S30" s="35">
         <v>338700000</v>
       </c>
-      <c r="T30" s="29">
+      <c r="T30" s="28">
         <v>11628.425956761619</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="B31" s="31">
+      <c r="B31" s="30">
         <v>67.892896174863381</v>
       </c>
-      <c r="C31" s="39">
+      <c r="C31" s="35">
         <v>1085100000</v>
       </c>
-      <c r="D31" s="28">
+      <c r="D31" s="27">
         <v>43668.104697208721</v>
       </c>
-      <c r="Q31" s="24" t="s">
+      <c r="Q31" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="R31" s="31"/>
-      <c r="S31" s="39"/>
-      <c r="T31" s="28">
+      <c r="R31" s="30"/>
+      <c r="S31" s="35"/>
+      <c r="T31" s="27">
         <v>43668.104697208721</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="B32" s="31">
+      <c r="B32" s="30">
         <v>156.51639344262296</v>
       </c>
-      <c r="C32" s="39">
+      <c r="C32" s="35">
         <v>213348333.33333337</v>
       </c>
-      <c r="D32" s="28">
+      <c r="D32" s="27">
         <v>3724.331558581363</v>
       </c>
-      <c r="Q32" s="24" t="s">
+      <c r="Q32" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="R32" s="31"/>
-      <c r="S32" s="39"/>
-      <c r="T32" s="28">
+      <c r="R32" s="30">
+        <v>156.51639344262296</v>
+      </c>
+      <c r="S32" s="35">
+        <v>213348333.33333337</v>
+      </c>
+      <c r="T32" s="27">
         <v>3724.331558581363</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="29"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="28"/>
       <c r="Q33" s="2"/>
-      <c r="R33" s="30"/>
-      <c r="S33" s="39"/>
-      <c r="T33" s="29"/>
+      <c r="R33" s="29"/>
+      <c r="S33" s="35"/>
+      <c r="T33" s="28"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B34" s="30">
+      <c r="B34" s="29">
         <v>69.928961748633881</v>
       </c>
-      <c r="C34" s="39">
+      <c r="C34" s="35">
         <v>1072223000</v>
       </c>
-      <c r="D34" s="29">
+      <c r="D34" s="28">
         <v>41893.529733531293</v>
       </c>
       <c r="Q34" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="R34" s="30"/>
-      <c r="S34" s="39"/>
-      <c r="T34" s="29">
+      <c r="R34" s="29"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="28">
         <v>41893.529733531293</v>
       </c>
     </row>
@@ -10924,25 +11952,25 @@
       <c r="A35" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="B35" s="30">
+      <c r="B35" s="29">
         <v>81.034672131147531</v>
       </c>
-      <c r="C35" s="39">
+      <c r="C35" s="35">
         <v>132875000</v>
       </c>
-      <c r="D35" s="29">
+      <c r="D35" s="28">
         <v>4480.1371874482656</v>
       </c>
       <c r="Q35" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="R35" s="30">
+      <c r="R35" s="29">
         <v>81.034672131147531</v>
       </c>
-      <c r="S35" s="39">
+      <c r="S35" s="35">
         <v>132875000</v>
       </c>
-      <c r="T35" s="29">
+      <c r="T35" s="28">
         <v>4480.1371874482656</v>
       </c>
     </row>
@@ -10950,25 +11978,25 @@
       <c r="A36" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B36" s="30">
+      <c r="B36" s="29">
         <v>69.928961748633881</v>
       </c>
-      <c r="C36" s="39">
+      <c r="C36" s="35">
         <v>100610000</v>
       </c>
-      <c r="D36" s="29">
+      <c r="D36" s="28">
         <v>3930.9994529967962</v>
       </c>
       <c r="Q36" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="R36" s="30">
+      <c r="R36" s="29">
         <v>69.928961748633881</v>
       </c>
-      <c r="S36" s="39">
+      <c r="S36" s="35">
         <v>100610000</v>
       </c>
-      <c r="T36" s="29">
+      <c r="T36" s="28">
         <v>3930.9994529967962</v>
       </c>
     </row>
@@ -10976,25 +12004,25 @@
       <c r="A37" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B37" s="30">
+      <c r="B37" s="29">
         <v>12.824999999999999</v>
       </c>
-      <c r="C37" s="39">
+      <c r="C37" s="35">
         <v>47796306</v>
       </c>
-      <c r="D37" s="29">
+      <c r="D37" s="28">
         <v>10182.534113060428</v>
       </c>
       <c r="Q37" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="R37" s="30">
+      <c r="R37" s="29">
         <v>12.824999999999999</v>
       </c>
-      <c r="S37" s="39">
+      <c r="S37" s="35">
         <v>47796306</v>
       </c>
-      <c r="T37" s="29">
+      <c r="T37" s="28">
         <v>10182.534113060428</v>
       </c>
     </row>
@@ -11002,25 +12030,25 @@
       <c r="A38" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B38" s="30">
+      <c r="B38" s="29">
         <v>26.721420765027325</v>
       </c>
-      <c r="C38" s="39">
+      <c r="C38" s="35">
         <v>260120703.40000001</v>
       </c>
-      <c r="D38" s="29">
+      <c r="D38" s="28">
         <v>26597.10015500959</v>
       </c>
       <c r="Q38" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="R38" s="30">
+      <c r="R38" s="29">
         <v>26.721420765027325</v>
       </c>
-      <c r="S38" s="39">
+      <c r="S38" s="35">
         <v>260120703.40000001</v>
       </c>
-      <c r="T38" s="29">
+      <c r="T38" s="28">
         <v>26597.10015500959</v>
       </c>
     </row>
@@ -11028,25 +12056,25 @@
       <c r="A39" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B39" s="30">
+      <c r="B39" s="29">
         <v>143.5311475409836</v>
       </c>
-      <c r="C39" s="39">
+      <c r="C39" s="35">
         <v>1054080000</v>
       </c>
-      <c r="D39" s="29">
+      <c r="D39" s="28">
         <v>20065.331109943578</v>
       </c>
       <c r="Q39" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="R39" s="30">
+      <c r="R39" s="29">
         <v>143.5311475409836</v>
       </c>
-      <c r="S39" s="39">
+      <c r="S39" s="35">
         <v>1054080000</v>
       </c>
-      <c r="T39" s="29">
+      <c r="T39" s="28">
         <v>20065.331109943578</v>
       </c>
     </row>
@@ -11054,25 +12082,25 @@
       <c r="A40" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B40" s="30">
+      <c r="B40" s="29">
         <v>30.396639344262294</v>
       </c>
-      <c r="C40" s="39">
+      <c r="C40" s="35">
         <v>109251549</v>
       </c>
-      <c r="D40" s="29">
+      <c r="D40" s="28">
         <v>9820.2138933607312</v>
       </c>
       <c r="Q40" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="R40" s="30">
+      <c r="R40" s="29">
         <v>30.396639344262294</v>
       </c>
-      <c r="S40" s="39">
+      <c r="S40" s="35">
         <v>109251549</v>
       </c>
-      <c r="T40" s="29">
+      <c r="T40" s="28">
         <v>9820.2138933607312</v>
       </c>
     </row>
@@ -11080,25 +12108,25 @@
       <c r="A41" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B41" s="30">
+      <c r="B41" s="29">
         <v>146.98128415300548</v>
       </c>
-      <c r="C41" s="39">
+      <c r="C41" s="35">
         <v>230512400</v>
       </c>
-      <c r="D41" s="29">
+      <c r="D41" s="28">
         <v>4285.0033878518789</v>
       </c>
       <c r="Q41" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="R41" s="30">
+      <c r="R41" s="29">
         <v>146.98128415300548</v>
       </c>
-      <c r="S41" s="39">
+      <c r="S41" s="35">
         <v>230512400</v>
       </c>
-      <c r="T41" s="29">
+      <c r="T41" s="28">
         <v>4285.0033878518789</v>
       </c>
     </row>
@@ -11106,25 +12134,25 @@
       <c r="A42" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B42" s="30">
+      <c r="B42" s="29">
         <v>107.19683057377048</v>
       </c>
-      <c r="C42" s="39">
+      <c r="C42" s="35">
         <v>515209333.33333337</v>
       </c>
-      <c r="D42" s="29">
+      <c r="D42" s="28">
         <v>13131.69210880782</v>
       </c>
       <c r="Q42" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="R42" s="30">
+      <c r="R42" s="29">
         <v>107.19683057377048</v>
       </c>
-      <c r="S42" s="39">
+      <c r="S42" s="35">
         <v>515209333.33333337</v>
       </c>
-      <c r="T42" s="29">
+      <c r="T42" s="28">
         <v>13131.69210880782</v>
       </c>
     </row>
@@ -11132,25 +12160,25 @@
       <c r="A43" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="B43" s="30">
+      <c r="B43" s="29">
         <v>5.7762420765027329</v>
       </c>
-      <c r="C43" s="39">
+      <c r="C43" s="35">
         <v>22684790</v>
       </c>
-      <c r="D43" s="29">
+      <c r="D43" s="28">
         <v>10730.211740705734</v>
       </c>
       <c r="Q43" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="R43" s="30">
+      <c r="R43" s="29">
         <v>5.7762420765027329</v>
       </c>
-      <c r="S43" s="39">
+      <c r="S43" s="35">
         <v>22684790</v>
       </c>
-      <c r="T43" s="29">
+      <c r="T43" s="28">
         <v>10730.211740705734</v>
       </c>
     </row>
@@ -11158,25 +12186,25 @@
       <c r="A44" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B44" s="30">
+      <c r="B44" s="29">
         <v>102.19631147540983</v>
       </c>
-      <c r="C44" s="39">
+      <c r="C44" s="35">
         <v>525983532</v>
       </c>
-      <c r="D44" s="29">
+      <c r="D44" s="28">
         <v>14062.283214161109</v>
       </c>
       <c r="Q44" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="R44" s="30">
+      <c r="R44" s="29">
         <v>102.19631147540983</v>
       </c>
-      <c r="S44" s="39">
+      <c r="S44" s="35">
         <v>525983532</v>
       </c>
-      <c r="T44" s="29">
+      <c r="T44" s="28">
         <v>14062.283214161109</v>
       </c>
     </row>
@@ -11184,25 +12212,25 @@
       <c r="A45" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B45" s="30">
+      <c r="B45" s="29">
         <v>33.748770491803278</v>
       </c>
-      <c r="C45" s="39">
+      <c r="C45" s="35">
         <v>229510953.33333334</v>
       </c>
-      <c r="D45" s="29">
+      <c r="D45" s="28">
         <v>18580.798598883048</v>
       </c>
       <c r="Q45" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="R45" s="30">
+      <c r="R45" s="29">
         <v>33.748770491803278</v>
       </c>
-      <c r="S45" s="39">
+      <c r="S45" s="35">
         <v>229510953.33333334</v>
       </c>
-      <c r="T45" s="29">
+      <c r="T45" s="28">
         <v>18580.798598883048</v>
       </c>
     </row>
@@ -11210,25 +12238,25 @@
       <c r="A46" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B46" s="30">
+      <c r="B46" s="29">
         <v>57.201092896174856</v>
       </c>
-      <c r="C46" s="39">
+      <c r="C46" s="35">
         <v>198866597</v>
       </c>
-      <c r="D46" s="29">
+      <c r="D46" s="28">
         <v>9498.9681212862306</v>
       </c>
       <c r="Q46" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="R46" s="30">
+      <c r="R46" s="29">
         <v>57.201092896174856</v>
       </c>
-      <c r="S46" s="39">
+      <c r="S46" s="35">
         <v>198866597</v>
       </c>
-      <c r="T46" s="29">
+      <c r="T46" s="28">
         <v>9498.9681212862306</v>
       </c>
     </row>
@@ -11236,25 +12264,25 @@
       <c r="A47" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B47" s="30">
+      <c r="B47" s="29">
         <v>2.3617759562841529</v>
       </c>
-      <c r="C47" s="39">
+      <c r="C47" s="35">
         <v>12270048</v>
       </c>
-      <c r="D47" s="29">
+      <c r="D47" s="28">
         <v>14194.708529517244</v>
       </c>
       <c r="Q47" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="R47" s="30">
+      <c r="R47" s="29">
         <v>2.3617759562841529</v>
       </c>
-      <c r="S47" s="39">
+      <c r="S47" s="35">
         <v>12270048</v>
       </c>
-      <c r="T47" s="29">
+      <c r="T47" s="28">
         <v>14194.708529517244</v>
       </c>
     </row>
@@ -11262,47 +12290,47 @@
       <c r="A48" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B48" s="30">
+      <c r="B48" s="29">
         <v>59.612021857923494</v>
       </c>
-      <c r="C48" s="39">
+      <c r="C48" s="35">
         <v>222437605</v>
       </c>
-      <c r="D48" s="29">
+      <c r="D48" s="28">
         <v>10195.141855348795</v>
       </c>
       <c r="Q48" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="R48" s="30">
+      <c r="R48" s="29">
         <v>59.612021857923494</v>
       </c>
-      <c r="S48" s="39">
+      <c r="S48" s="35">
         <v>222437605</v>
       </c>
-      <c r="T48" s="29">
+      <c r="T48" s="28">
         <v>10195.141855348795</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="B49" s="31">
+      <c r="B49" s="30">
         <v>3.4076502732240437</v>
       </c>
-      <c r="C49" s="39">
+      <c r="C49" s="35">
         <v>73200000</v>
       </c>
-      <c r="D49" s="28">
+      <c r="D49" s="27">
         <v>58691.468890314303</v>
       </c>
-      <c r="Q49" s="24" t="s">
+      <c r="Q49" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="R49" s="31"/>
-      <c r="S49" s="39"/>
-      <c r="T49" s="28">
+      <c r="R49" s="30"/>
+      <c r="S49" s="35"/>
+      <c r="T49" s="27">
         <v>58691.468890314303</v>
       </c>
     </row>
@@ -11310,25 +12338,25 @@
       <c r="A50" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B50" s="30">
+      <c r="B50" s="29">
         <v>22.460655737704919</v>
       </c>
-      <c r="C50" s="39">
+      <c r="C50" s="35">
         <v>76583333.333333343</v>
       </c>
-      <c r="D50" s="29">
+      <c r="D50" s="28">
         <v>9316.0272161804896</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="R50" s="30">
+      <c r="R50" s="29">
         <v>22.460655737704919</v>
       </c>
-      <c r="S50" s="39">
+      <c r="S50" s="35">
         <v>76583333.333333343</v>
       </c>
-      <c r="T50" s="29">
+      <c r="T50" s="28">
         <v>9316.0272161804896</v>
       </c>
     </row>
@@ -11336,25 +12364,25 @@
       <c r="A51" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B51" s="30">
+      <c r="B51" s="29">
         <v>33.089344262295086</v>
       </c>
-      <c r="C51" s="39">
+      <c r="C51" s="35">
         <v>20184500.000000004</v>
       </c>
-      <c r="D51" s="29">
+      <c r="D51" s="28">
         <v>1666.666666666667</v>
       </c>
       <c r="Q51" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="R51" s="30">
+      <c r="R51" s="29">
         <v>33.089344262295086</v>
       </c>
-      <c r="S51" s="39">
+      <c r="S51" s="35">
         <v>20184500.000000004</v>
       </c>
-      <c r="T51" s="29">
+      <c r="T51" s="28">
         <v>1666.666666666667</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Calculate Chini R2 and clean up code
</commit_message>
<xml_diff>
--- a/01_raw_data/chini-biogas/chini_biogas-data.xlsx
+++ b/01_raw_data/chini-biogas/chini_biogas-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sahar/Documents/methane_letter/01_raw_data/chini-biogas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8466111D-8EB3-4B4F-95EF-04ABCF91F02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB56300-39A3-1E49-93BF-DD655B8B24C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="520" windowWidth="31980" windowHeight="21080" activeTab="1" xr2:uid="{E612D14B-5A41-9848-9237-46E1EE074146}"/>
+    <workbookView xWindow="2080" yWindow="520" windowWidth="35880" windowHeight="21080" activeTab="6" xr2:uid="{E612D14B-5A41-9848-9237-46E1EE074146}"/>
   </bookViews>
   <sheets>
     <sheet name="All data" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Biogas Col Key" sheetId="3" r:id="rId4"/>
     <sheet name="Unit conversions" sheetId="4" r:id="rId5"/>
     <sheet name="Plotting" sheetId="5" r:id="rId6"/>
+    <sheet name="Testing plot R2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="402">
   <si>
     <t>CWNS ID</t>
   </si>
@@ -3036,6 +3037,1542 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>All Data</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Testing plot R2'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>biogas_2012_scf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="50"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-AB3A-C94F-B1C4-7070C3527CA1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.0278019553468416E-2"/>
+                  <c:y val="-2.3786763141093917E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Testing plot R2'!$B$2:$B$52</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>56.436311475409831</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.279748633879784</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.633737704918033</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>131.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.070573770491803</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.470956284153004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>112.87978142076503</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.9833333333333334</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.720765027322404</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>614.6994535519126</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>125.63005867459017</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35.712158469945351</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28.652732240437157</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.976256830601095</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.3424043715847001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41.536532704918031</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.990642076502732</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>46.954644808743176</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5017759562841528</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.7553005464480878</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.2807103825136616</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>39.415573770491804</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.76937081967213</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.248712382513661</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>104.3004918032787</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>36.641374316939888</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>36.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>79.581693989071042</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>67.892896174863381</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>156.51639344262296</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>69.928961748633881</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>81.034672131147531</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>69.928961748633881</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>12.824999999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>26.721420765027325</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>143.5311475409836</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>30.396639344262294</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>146.98128415300548</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>107.19683057377048</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.7762420765027329</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>102.19631147540983</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>33.748770491803278</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>57.201092896174856</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.3617759562841529</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>59.612021857923494</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.4076502732240437</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>22.460655737704919</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>33.089344262295086</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Testing plot R2'!$C$2:$C$52</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="1">
+                  <c:v>137991378.20000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59659000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4021242000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>86030950</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49347000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>174134200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18554666.666666668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>76264666.666666672</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>182193666.66666669</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>968752819.45899999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>206329392</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>121391220</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>78667674</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29680770</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>159260997.59999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>51331878</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>284977500</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3709528</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22284115</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>38351800</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>236718970</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>133967709.40000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6468208.7000000002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>415332388.10000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>331468584.19999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>331360000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>338700000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1085100000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>213348333.33333337</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1072223000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>132875000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>100610000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>47796306</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>260120703.40000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1054080000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>109251549</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>230512400</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>515209333.33333337</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>22684790</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>525983532</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>229510953.33333334</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>198866597</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>12270048</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>222437605</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>73200000</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>76583333.333333343</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20184500.000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AB3A-C94F-B1C4-7070C3527CA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="377404111"/>
+        <c:axId val="488357087"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="377404111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Facility Size (MGD)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488357087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="488357087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Biogas Production (SCF)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="377404111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Remove Extreme Outliers</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Testing plot R2'!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>biogas_2012_scf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.0278019553468416E-2"/>
+                  <c:y val="-2.3786763141093917E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Testing plot R2'!$R$2:$R$43</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>33.279748633879784</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.633737704918033</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.070573770491803</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.470956284153004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112.87978142076503</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.9833333333333334</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.720765027322404</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125.63005867459017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35.712158469945351</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.652732240437157</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.976256830601095</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.3424043715847001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41.536532704918031</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.990642076502732</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>46.954644808743176</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5017759562841528</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.7553005464480878</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.2807103825136616</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39.415573770491804</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23.76937081967213</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.248712382513661</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>104.3004918032787</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>36.641374316939888</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>36.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>79.581693989071042</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>156.51639344262296</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>81.034672131147531</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>69.928961748633881</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12.824999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>26.721420765027325</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>143.5311475409836</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>30.396639344262294</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>146.98128415300548</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>107.19683057377048</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.7762420765027329</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>102.19631147540983</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>33.748770491803278</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>57.201092896174856</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.3617759562841529</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>59.612021857923494</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>22.460655737704919</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>33.089344262295086</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Testing plot R2'!$S$2:$S$43</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>137991378.20000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59659000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86030950</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49347000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>174134200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18554666.666666668</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76264666.666666672</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>968752819.45899999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>206329392</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>121391220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>78667674</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29680770</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>159260997.59999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>51331878</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>284977500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3709528</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22284115</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>38351800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>236718970</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>133967709.40000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6468208.7000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>415332388.10000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>331468584.19999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>331360000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>338700000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>213348333.33333337</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>132875000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>100610000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>47796306</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>260120703.40000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1054080000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>109251549</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>230512400</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>515209333.33333337</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>22684790</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>525983532</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>229510953.33333334</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>198866597</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12270048</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>222437605</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>76583333.333333343</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20184500.000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1A0F-8D45-91DE-C0523F6AA570}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="377404111"/>
+        <c:axId val="488357087"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="377404111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Facility Size (MGD)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488357087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="488357087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Biogas Production (SCF)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="377404111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3077,6 +4614,86 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4074,6 +5691,964 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4131,6 +6706,87 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EBA0B2B-69D9-3843-8AB7-B5510DC127D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53DE0CD8-814D-624D-B040-7347C5854CF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AE39691-CD4E-A349-A13F-C0C74372357D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8175,8 +10831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1169CC32-FE8E-0247-8B6B-8C48D3D455D8}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView topLeftCell="A18" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11105,7 +13761,7 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12390,4 +15046,1240 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BC3A8F-E0C9-5D47-9B95-70C3C8079C3F}">
+  <dimension ref="A1:T51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="R45" sqref="R45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" style="35" customWidth="1"/>
+    <col min="17" max="17" width="16.1640625" customWidth="1"/>
+    <col min="18" max="18" width="24.1640625" style="35" customWidth="1"/>
+    <col min="19" max="19" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.83203125" style="35" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>391</v>
+      </c>
+      <c r="C1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="R1" s="32" t="s">
+        <v>391</v>
+      </c>
+      <c r="S1" t="s">
+        <v>366</v>
+      </c>
+      <c r="T1" s="32" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="29">
+        <v>56.436311475409831</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="29"/>
+      <c r="Q2" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="29">
+        <v>33.279748633879784</v>
+      </c>
+      <c r="S2" s="35">
+        <v>137991378.20000002</v>
+      </c>
+      <c r="T2" s="29">
+        <v>11328.980505382917</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="29">
+        <v>33.279748633879784</v>
+      </c>
+      <c r="C3" s="35">
+        <v>137991378.20000002</v>
+      </c>
+      <c r="D3" s="29">
+        <v>11328.980505382917</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="29">
+        <v>13.633737704918033</v>
+      </c>
+      <c r="S3" s="35">
+        <v>59659000</v>
+      </c>
+      <c r="T3" s="29">
+        <v>11955.836012719972</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="29">
+        <v>13.633737704918033</v>
+      </c>
+      <c r="C4" s="35">
+        <v>59659000</v>
+      </c>
+      <c r="D4" s="29">
+        <v>11955.836012719972</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="R4" s="29">
+        <v>15.070573770491803</v>
+      </c>
+      <c r="S4" s="35">
+        <v>86030950</v>
+      </c>
+      <c r="T4" s="29">
+        <v>15597.099620546682</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="30">
+        <v>131.9</v>
+      </c>
+      <c r="C5" s="35">
+        <v>4021242000</v>
+      </c>
+      <c r="D5" s="30">
+        <v>83297.95299469294</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="R5" s="29">
+        <v>12.470956284153004</v>
+      </c>
+      <c r="S5" s="35">
+        <v>49347000</v>
+      </c>
+      <c r="T5" s="29">
+        <v>10811.349649568287</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="29">
+        <v>15.070573770491803</v>
+      </c>
+      <c r="C6" s="35">
+        <v>86030950</v>
+      </c>
+      <c r="D6" s="29">
+        <v>15597.099620546682</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R6" s="29">
+        <v>112.87978142076503</v>
+      </c>
+      <c r="S6" s="35">
+        <v>174134200</v>
+      </c>
+      <c r="T6" s="29">
+        <v>4214.8956770102141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="29">
+        <v>12.470956284153004</v>
+      </c>
+      <c r="C7" s="35">
+        <v>49347000</v>
+      </c>
+      <c r="D7" s="29">
+        <v>10811.349649568287</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="R7" s="29">
+        <v>7.9833333333333334</v>
+      </c>
+      <c r="S7" s="35">
+        <v>18554666.666666668</v>
+      </c>
+      <c r="T7" s="28">
+        <v>6350.2059162417154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="29">
+        <v>112.87978142076503</v>
+      </c>
+      <c r="C8" s="35">
+        <v>174134200</v>
+      </c>
+      <c r="D8" s="29">
+        <v>4214.8956770102141</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="R8" s="29">
+        <v>23.720765027322404</v>
+      </c>
+      <c r="S8" s="35">
+        <v>76264666.666666672</v>
+      </c>
+      <c r="T8" s="28">
+        <v>8784.430264077344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="29">
+        <v>7.9833333333333334</v>
+      </c>
+      <c r="C9" s="35">
+        <v>18554666.666666668</v>
+      </c>
+      <c r="D9" s="28">
+        <v>6350.2059162417154</v>
+      </c>
+      <c r="Q9" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="R9" s="30">
+        <v>125.63005867459017</v>
+      </c>
+      <c r="S9" s="35">
+        <v>968752819.45899999</v>
+      </c>
+      <c r="T9" s="27">
+        <v>21068.728733090302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="29">
+        <v>23.720765027322404</v>
+      </c>
+      <c r="C10" s="35">
+        <v>76264666.666666672</v>
+      </c>
+      <c r="D10" s="28">
+        <v>8784.430264077344</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="R10" s="29">
+        <v>35.712158469945351</v>
+      </c>
+      <c r="S10" s="35">
+        <v>206329392</v>
+      </c>
+      <c r="T10" s="28">
+        <v>15785.702470802906</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="30">
+        <v>614.6994535519126</v>
+      </c>
+      <c r="C11" s="34">
+        <v>182193666.66666669</v>
+      </c>
+      <c r="D11" s="27">
+        <v>809.82161377307625</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="R11" s="29">
+        <v>28.652732240437157</v>
+      </c>
+      <c r="S11" s="35">
+        <v>121391220</v>
+      </c>
+      <c r="T11" s="28">
+        <v>11575.510398687888</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="30">
+        <v>125.63005867459017</v>
+      </c>
+      <c r="C12" s="35">
+        <v>968752819.45899999</v>
+      </c>
+      <c r="D12" s="27">
+        <v>21068.728733090302</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="R12" s="29">
+        <v>18.976256830601095</v>
+      </c>
+      <c r="S12" s="35">
+        <v>78667674</v>
+      </c>
+      <c r="T12" s="28">
+        <v>11326.73329196249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="29">
+        <v>35.712158469945351</v>
+      </c>
+      <c r="C13" s="35">
+        <v>206329392</v>
+      </c>
+      <c r="D13" s="28">
+        <v>15785.702470802906</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="R13" s="29">
+        <v>6.3424043715847001</v>
+      </c>
+      <c r="S13" s="35">
+        <v>29680770</v>
+      </c>
+      <c r="T13" s="28">
+        <v>12786.160460427687</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="29">
+        <v>28.652732240437157</v>
+      </c>
+      <c r="C14" s="35">
+        <v>121391220</v>
+      </c>
+      <c r="D14" s="28">
+        <v>11575.510398687888</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="R14" s="29">
+        <v>41.536532704918031</v>
+      </c>
+      <c r="S14" s="35">
+        <v>159260997.59999999</v>
+      </c>
+      <c r="T14" s="28">
+        <v>10476.063103201592</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="29">
+        <v>18.976256830601095</v>
+      </c>
+      <c r="C15" s="35">
+        <v>78667674</v>
+      </c>
+      <c r="D15" s="28">
+        <v>11326.73329196249</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="R15" s="29">
+        <v>11.990642076502732</v>
+      </c>
+      <c r="S15" s="35">
+        <v>51331878</v>
+      </c>
+      <c r="T15" s="28">
+        <v>11696.70747338259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="29">
+        <v>6.3424043715847001</v>
+      </c>
+      <c r="C16" s="35">
+        <v>29680770</v>
+      </c>
+      <c r="D16" s="28">
+        <v>12786.160460427687</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="R16" s="29">
+        <v>46.954644808743176</v>
+      </c>
+      <c r="S16" s="35">
+        <v>284977500</v>
+      </c>
+      <c r="T16" s="28">
+        <v>16582.53517520686</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="29">
+        <v>41.536532704918031</v>
+      </c>
+      <c r="C17" s="35">
+        <v>159260997.59999999</v>
+      </c>
+      <c r="D17" s="28">
+        <v>10476.063103201592</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="R17" s="29">
+        <v>1.5017759562841528</v>
+      </c>
+      <c r="S17" s="35">
+        <v>3709528</v>
+      </c>
+      <c r="T17" s="28">
+        <v>6748.8911125261529</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="29">
+        <v>11.990642076502732</v>
+      </c>
+      <c r="C18" s="35">
+        <v>51331878</v>
+      </c>
+      <c r="D18" s="28">
+        <v>11696.70747338259</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="R18" s="29">
+        <v>3.7553005464480878</v>
+      </c>
+      <c r="S18" s="35">
+        <v>22284115</v>
+      </c>
+      <c r="T18" s="28">
+        <v>16213.232298245102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="29">
+        <v>46.954644808743176</v>
+      </c>
+      <c r="C19" s="35">
+        <v>284977500</v>
+      </c>
+      <c r="D19" s="28">
+        <v>16582.53517520686</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="R19" s="29">
+        <v>5.2807103825136616</v>
+      </c>
+      <c r="S19" s="35">
+        <v>38351800</v>
+      </c>
+      <c r="T19" s="28">
+        <v>19843.227749205791</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="29">
+        <v>1.5017759562841528</v>
+      </c>
+      <c r="C20" s="35">
+        <v>3709528</v>
+      </c>
+      <c r="D20" s="28">
+        <v>6748.8911125261529</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="R20" s="29">
+        <v>39.415573770491804</v>
+      </c>
+      <c r="S20" s="35">
+        <v>236718970</v>
+      </c>
+      <c r="T20" s="28">
+        <v>16409.075911022384</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" s="29">
+        <v>3.7553005464480878</v>
+      </c>
+      <c r="C21" s="35">
+        <v>22284115</v>
+      </c>
+      <c r="D21" s="28">
+        <v>16213.232298245102</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="R21" s="29">
+        <v>23.76937081967213</v>
+      </c>
+      <c r="S21" s="35">
+        <v>133967709.40000001</v>
+      </c>
+      <c r="T21" s="28">
+        <v>15399.313497740444</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" s="29">
+        <v>5.2807103825136616</v>
+      </c>
+      <c r="C22" s="35">
+        <v>38351800</v>
+      </c>
+      <c r="D22" s="28">
+        <v>19843.227749205791</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="R22" s="29">
+        <v>2.248712382513661</v>
+      </c>
+      <c r="S22" s="35">
+        <v>6468208.7000000002</v>
+      </c>
+      <c r="T22" s="28">
+        <v>7859.0314633146982</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="28"/>
+      <c r="Q23" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="R23" s="29">
+        <v>104.3004918032787</v>
+      </c>
+      <c r="S23" s="35">
+        <v>415332388.10000002</v>
+      </c>
+      <c r="T23" s="28">
+        <v>10879.986527472378</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" s="29">
+        <v>39.415573770491804</v>
+      </c>
+      <c r="C24" s="35">
+        <v>236718970</v>
+      </c>
+      <c r="D24" s="28">
+        <v>16409.075911022384</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="R24" s="29">
+        <v>36.641374316939888</v>
+      </c>
+      <c r="S24" s="35">
+        <v>331468584.19999999</v>
+      </c>
+      <c r="T24" s="28">
+        <v>24716.645766755799</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B25" s="29">
+        <v>23.76937081967213</v>
+      </c>
+      <c r="C25" s="35">
+        <v>133967709.40000001</v>
+      </c>
+      <c r="D25" s="28">
+        <v>15399.313497740444</v>
+      </c>
+      <c r="Q25" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="R25" s="29">
+        <v>36.666666666666664</v>
+      </c>
+      <c r="S25" s="35">
+        <v>331360000</v>
+      </c>
+      <c r="T25" s="28">
+        <v>24691.505216095378</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" s="29">
+        <v>2.248712382513661</v>
+      </c>
+      <c r="C26" s="35">
+        <v>6468208.7000000002</v>
+      </c>
+      <c r="D26" s="28">
+        <v>7859.0314633146982</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="R26" s="29">
+        <v>79.581693989071042</v>
+      </c>
+      <c r="S26" s="35">
+        <v>338700000</v>
+      </c>
+      <c r="T26" s="28">
+        <v>11628.425956761619</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B27" s="29">
+        <v>104.3004918032787</v>
+      </c>
+      <c r="C27" s="35">
+        <v>415332388.10000002</v>
+      </c>
+      <c r="D27" s="28">
+        <v>10879.986527472378</v>
+      </c>
+      <c r="Q27" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="R27" s="30">
+        <v>156.51639344262296</v>
+      </c>
+      <c r="S27" s="35">
+        <v>213348333.33333337</v>
+      </c>
+      <c r="T27" s="27">
+        <v>3724.331558581363</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B28" s="29">
+        <v>36.641374316939888</v>
+      </c>
+      <c r="C28" s="35">
+        <v>331468584.19999999</v>
+      </c>
+      <c r="D28" s="28">
+        <v>24716.645766755799</v>
+      </c>
+      <c r="Q28" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="R28" s="29">
+        <v>81.034672131147531</v>
+      </c>
+      <c r="S28" s="35">
+        <v>132875000</v>
+      </c>
+      <c r="T28" s="28">
+        <v>4480.1371874482656</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B29" s="29">
+        <v>36.666666666666664</v>
+      </c>
+      <c r="C29" s="35">
+        <v>331360000</v>
+      </c>
+      <c r="D29" s="28">
+        <v>24691.505216095378</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="R29" s="29">
+        <v>69.928961748633881</v>
+      </c>
+      <c r="S29" s="35">
+        <v>100610000</v>
+      </c>
+      <c r="T29" s="28">
+        <v>3930.9994529967962</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" s="29">
+        <v>79.581693989071042</v>
+      </c>
+      <c r="C30" s="35">
+        <v>338700000</v>
+      </c>
+      <c r="D30" s="28">
+        <v>11628.425956761619</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="R30" s="29">
+        <v>12.824999999999999</v>
+      </c>
+      <c r="S30" s="35">
+        <v>47796306</v>
+      </c>
+      <c r="T30" s="28">
+        <v>10182.534113060428</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A31" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" s="30">
+        <v>67.892896174863381</v>
+      </c>
+      <c r="C31" s="35">
+        <v>1085100000</v>
+      </c>
+      <c r="D31" s="27">
+        <v>43668.104697208721</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="R31" s="29">
+        <v>26.721420765027325</v>
+      </c>
+      <c r="S31" s="35">
+        <v>260120703.40000001</v>
+      </c>
+      <c r="T31" s="28">
+        <v>26597.10015500959</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A32" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="B32" s="30">
+        <v>156.51639344262296</v>
+      </c>
+      <c r="C32" s="35">
+        <v>213348333.33333337</v>
+      </c>
+      <c r="D32" s="27">
+        <v>3724.331558581363</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="R32" s="29">
+        <v>143.5311475409836</v>
+      </c>
+      <c r="S32" s="35">
+        <v>1054080000</v>
+      </c>
+      <c r="T32" s="28">
+        <v>20065.331109943578</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="28"/>
+      <c r="Q33" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="R33" s="29">
+        <v>30.396639344262294</v>
+      </c>
+      <c r="S33" s="35">
+        <v>109251549</v>
+      </c>
+      <c r="T33" s="28">
+        <v>9820.2138933607312</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B34" s="29">
+        <v>69.928961748633881</v>
+      </c>
+      <c r="C34" s="35">
+        <v>1072223000</v>
+      </c>
+      <c r="D34" s="28">
+        <v>41893.529733531293</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="R34" s="29">
+        <v>146.98128415300548</v>
+      </c>
+      <c r="S34" s="35">
+        <v>230512400</v>
+      </c>
+      <c r="T34" s="28">
+        <v>4285.0033878518789</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B35" s="29">
+        <v>81.034672131147531</v>
+      </c>
+      <c r="C35" s="35">
+        <v>132875000</v>
+      </c>
+      <c r="D35" s="28">
+        <v>4480.1371874482656</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="R35" s="29">
+        <v>107.19683057377048</v>
+      </c>
+      <c r="S35" s="35">
+        <v>515209333.33333337</v>
+      </c>
+      <c r="T35" s="28">
+        <v>13131.69210880782</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B36" s="29">
+        <v>69.928961748633881</v>
+      </c>
+      <c r="C36" s="35">
+        <v>100610000</v>
+      </c>
+      <c r="D36" s="28">
+        <v>3930.9994529967962</v>
+      </c>
+      <c r="Q36" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="R36" s="29">
+        <v>5.7762420765027329</v>
+      </c>
+      <c r="S36" s="35">
+        <v>22684790</v>
+      </c>
+      <c r="T36" s="28">
+        <v>10730.211740705734</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B37" s="29">
+        <v>12.824999999999999</v>
+      </c>
+      <c r="C37" s="35">
+        <v>47796306</v>
+      </c>
+      <c r="D37" s="28">
+        <v>10182.534113060428</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="R37" s="29">
+        <v>102.19631147540983</v>
+      </c>
+      <c r="S37" s="35">
+        <v>525983532</v>
+      </c>
+      <c r="T37" s="28">
+        <v>14062.283214161109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B38" s="29">
+        <v>26.721420765027325</v>
+      </c>
+      <c r="C38" s="35">
+        <v>260120703.40000001</v>
+      </c>
+      <c r="D38" s="28">
+        <v>26597.10015500959</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="R38" s="29">
+        <v>33.748770491803278</v>
+      </c>
+      <c r="S38" s="35">
+        <v>229510953.33333334</v>
+      </c>
+      <c r="T38" s="28">
+        <v>18580.798598883048</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B39" s="29">
+        <v>143.5311475409836</v>
+      </c>
+      <c r="C39" s="35">
+        <v>1054080000</v>
+      </c>
+      <c r="D39" s="28">
+        <v>20065.331109943578</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="R39" s="29">
+        <v>57.201092896174856</v>
+      </c>
+      <c r="S39" s="35">
+        <v>198866597</v>
+      </c>
+      <c r="T39" s="28">
+        <v>9498.9681212862306</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B40" s="29">
+        <v>30.396639344262294</v>
+      </c>
+      <c r="C40" s="35">
+        <v>109251549</v>
+      </c>
+      <c r="D40" s="28">
+        <v>9820.2138933607312</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="R40" s="29">
+        <v>2.3617759562841529</v>
+      </c>
+      <c r="S40" s="35">
+        <v>12270048</v>
+      </c>
+      <c r="T40" s="28">
+        <v>14194.708529517244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B41" s="29">
+        <v>146.98128415300548</v>
+      </c>
+      <c r="C41" s="35">
+        <v>230512400</v>
+      </c>
+      <c r="D41" s="28">
+        <v>4285.0033878518789</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="R41" s="29">
+        <v>59.612021857923494</v>
+      </c>
+      <c r="S41" s="35">
+        <v>222437605</v>
+      </c>
+      <c r="T41" s="28">
+        <v>10195.141855348795</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B42" s="29">
+        <v>107.19683057377048</v>
+      </c>
+      <c r="C42" s="35">
+        <v>515209333.33333337</v>
+      </c>
+      <c r="D42" s="28">
+        <v>13131.69210880782</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="R42" s="29">
+        <v>22.460655737704919</v>
+      </c>
+      <c r="S42" s="35">
+        <v>76583333.333333343</v>
+      </c>
+      <c r="T42" s="28">
+        <v>9316.0272161804896</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B43" s="29">
+        <v>5.7762420765027329</v>
+      </c>
+      <c r="C43" s="35">
+        <v>22684790</v>
+      </c>
+      <c r="D43" s="28">
+        <v>10730.211740705734</v>
+      </c>
+      <c r="Q43" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="R43" s="29">
+        <v>33.089344262295086</v>
+      </c>
+      <c r="S43" s="35">
+        <v>20184500.000000004</v>
+      </c>
+      <c r="T43" s="28">
+        <v>1666.666666666667</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B44" s="29">
+        <v>102.19631147540983</v>
+      </c>
+      <c r="C44" s="35">
+        <v>525983532</v>
+      </c>
+      <c r="D44" s="28">
+        <v>14062.283214161109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B45" s="29">
+        <v>33.748770491803278</v>
+      </c>
+      <c r="C45" s="35">
+        <v>229510953.33333334</v>
+      </c>
+      <c r="D45" s="28">
+        <v>18580.798598883048</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B46" s="29">
+        <v>57.201092896174856</v>
+      </c>
+      <c r="C46" s="35">
+        <v>198866597</v>
+      </c>
+      <c r="D46" s="28">
+        <v>9498.9681212862306</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B47" s="29">
+        <v>2.3617759562841529</v>
+      </c>
+      <c r="C47" s="35">
+        <v>12270048</v>
+      </c>
+      <c r="D47" s="28">
+        <v>14194.708529517244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B48" s="29">
+        <v>59.612021857923494</v>
+      </c>
+      <c r="C48" s="35">
+        <v>222437605</v>
+      </c>
+      <c r="D48" s="28">
+        <v>10195.141855348795</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="B49" s="30">
+        <v>3.4076502732240437</v>
+      </c>
+      <c r="C49" s="35">
+        <v>73200000</v>
+      </c>
+      <c r="D49" s="27">
+        <v>58691.468890314303</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B50" s="29">
+        <v>22.460655737704919</v>
+      </c>
+      <c r="C50" s="35">
+        <v>76583333.333333343</v>
+      </c>
+      <c r="D50" s="28">
+        <v>9316.0272161804896</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B51" s="29">
+        <v>33.089344262295086</v>
+      </c>
+      <c r="C51" s="35">
+        <v>20184500.000000004</v>
+      </c>
+      <c r="D51" s="28">
+        <v>1666.666666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Make clean versions of benchmarking paper CHP and AD data
</commit_message>
<xml_diff>
--- a/01_raw_data/chini-biogas/chini_biogas-data.xlsx
+++ b/01_raw_data/chini-biogas/chini_biogas-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sahar/Documents/methane_letter/01_raw_data/chini-biogas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB56300-39A3-1E49-93BF-DD655B8B24C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CE6138-9F1A-254F-944C-83A18496992A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="520" windowWidth="35880" windowHeight="21080" activeTab="6" xr2:uid="{E612D14B-5A41-9848-9237-46E1EE074146}"/>
+    <workbookView xWindow="5600" yWindow="520" windowWidth="30080" windowHeight="21080" activeTab="4" xr2:uid="{E612D14B-5A41-9848-9237-46E1EE074146}"/>
   </bookViews>
   <sheets>
     <sheet name="All data" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="415">
   <si>
     <t>CWNS ID</t>
   </si>
@@ -1247,6 +1247,45 @@
   </si>
   <si>
     <t xml:space="preserve"> biogas_gen_value </t>
+  </si>
+  <si>
+    <t>137991378.20000002</t>
+  </si>
+  <si>
+    <t>17127384.615384616</t>
+  </si>
+  <si>
+    <t>70398153.84615384</t>
+  </si>
+  <si>
+    <t>196936923.07692307</t>
+  </si>
+  <si>
+    <t>475577846.15384614</t>
+  </si>
+  <si>
+    <t>211856264.6153846</t>
+  </si>
+  <si>
+    <t>18631846.153846152</t>
+  </si>
+  <si>
+    <t>excel_location</t>
+  </si>
+  <si>
+    <t>excel_facility_size_MGD</t>
+  </si>
+  <si>
+    <t>excel_biogas_2012_scf</t>
+  </si>
+  <si>
+    <t>py_location</t>
+  </si>
+  <si>
+    <t>py_facility_size_MGD</t>
+  </si>
+  <si>
+    <t>py_biogas_gen_scf</t>
   </si>
 </sst>
 </file>
@@ -1348,7 +1387,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1367,6 +1406,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1381,7 +1426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1480,6 +1525,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3934,7 +3987,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>biogas_2012_scf</c:v>
+                  <c:v>excel_biogas_2012_scf</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4377,6 +4430,732 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488357087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="488357087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Biogas Production (SCF)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="377404111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cleaned Chini Data</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>From Python</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Testing plot R2'!$V$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>py_biogas_gen_scf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.0278019553468416E-2"/>
+                  <c:y val="-2.3786763141093917E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Testing plot R2'!$U$2:$U$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>33.27974863</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.633737699999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.070573769999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.470956279999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112.8797814</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.983333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.720765029999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125.63005870000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35.712158469999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.652732239999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.976256830000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.3424043719999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41.536532700000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.990642080000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>46.954644809999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5017759559999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.755300546</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.2807103829999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39.415573770000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23.769370819999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.248712383</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>104.3004918</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>36.641374319999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>36.666666669999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>79.581693990000005</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>156.5163934</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>81.034672130000004</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>69.928961749999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12.824999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>26.721420770000002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>143.5311475</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>30.39663934</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>146.9812842</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>107.1968306</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.776242077</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>102.19631149999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>33.748770489999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>57.201092899999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.3617759559999998</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>59.612021859999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>22.46065574</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>33.089344259999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Testing plot R2'!$V$2:$V$43</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59659000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86030950</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49347000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>174134200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>968752819.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>206329392</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>121391220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>78667674</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29680770</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>159260997.59999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>51331878</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>284977500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3709528</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22284115</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>38351800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>236718970</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>133967709.40000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6468208.7000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>415332388.10000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>331468584.19999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>331360000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>338700000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>132875000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>100610000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>47796306</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>260120703.40000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1054080000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>109251549</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>230512400</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>22684790</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>525983532</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>198866597</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12270048</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>222437605</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>70692307.692307696</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DEF7-8C4F-B3BE-D253E1435080}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="377404111"/>
+        <c:axId val="488357087"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="377404111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Facility Size (MGD)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4694,6 +5473,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6649,6 +7468,485 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6801,6 +8099,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>693209</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>77258</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF3E0DDB-EA78-A24C-BF74-BA41192A7C52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10831,7 +12167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1169CC32-FE8E-0247-8B6B-8C48D3D455D8}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -13639,8 +14975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B12C50-DC4E-5D46-A39D-190792E41EE6}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15050,10 +16386,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BC3A8F-E0C9-5D47-9B95-70C3C8079C3F}">
-  <dimension ref="A1:T51"/>
+  <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="R45" sqref="R45"/>
+    <sheetView topLeftCell="K1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7:V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15065,10 +16401,12 @@
     <col min="17" max="17" width="16.1640625" customWidth="1"/>
     <col min="18" max="18" width="24.1640625" style="35" customWidth="1"/>
     <col min="19" max="19" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.83203125" style="35" customWidth="1"/>
+    <col min="20" max="20" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>359</v>
       </c>
@@ -15082,19 +16420,25 @@
         <v>380</v>
       </c>
       <c r="Q1" s="13" t="s">
-        <v>359</v>
+        <v>409</v>
       </c>
       <c r="R1" s="32" t="s">
-        <v>391</v>
+        <v>410</v>
       </c>
       <c r="S1" t="s">
-        <v>366</v>
-      </c>
-      <c r="T1" s="32" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>412</v>
+      </c>
+      <c r="U1" t="s">
+        <v>413</v>
+      </c>
+      <c r="V1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>25</v>
       </c>
@@ -15112,11 +16456,17 @@
       <c r="S2" s="35">
         <v>137991378.20000002</v>
       </c>
-      <c r="T2" s="29">
-        <v>11328.980505382917</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2">
+        <v>33.27974863</v>
+      </c>
+      <c r="V2" s="52" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>32</v>
       </c>
@@ -15138,11 +16488,17 @@
       <c r="S3" s="35">
         <v>59659000</v>
       </c>
-      <c r="T3" s="29">
-        <v>11955.836012719972</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T3" t="s">
+        <v>51</v>
+      </c>
+      <c r="U3">
+        <v>13.633737699999999</v>
+      </c>
+      <c r="V3" s="35">
+        <v>59659000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -15164,11 +16520,17 @@
       <c r="S4" s="35">
         <v>86030950</v>
       </c>
-      <c r="T4" s="29">
-        <v>15597.099620546682</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T4" t="s">
+        <v>69</v>
+      </c>
+      <c r="U4">
+        <v>15.070573769999999</v>
+      </c>
+      <c r="V4" s="35">
+        <v>86030950</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>55</v>
       </c>
@@ -15190,11 +16552,17 @@
       <c r="S5" s="35">
         <v>49347000</v>
       </c>
-      <c r="T5" s="29">
-        <v>10811.349649568287</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T5" t="s">
+        <v>69</v>
+      </c>
+      <c r="U5">
+        <v>12.470956279999999</v>
+      </c>
+      <c r="V5" s="35">
+        <v>49347000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>69</v>
       </c>
@@ -15216,11 +16584,17 @@
       <c r="S6" s="35">
         <v>174134200</v>
       </c>
-      <c r="T6" s="29">
-        <v>4214.8956770102141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T6" t="s">
+        <v>76</v>
+      </c>
+      <c r="U6">
+        <v>112.8797814</v>
+      </c>
+      <c r="V6" s="35">
+        <v>174134200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>69</v>
       </c>
@@ -15233,20 +16607,26 @@
       <c r="D7" s="29">
         <v>10811.349649568287</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="Q7" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="R7" s="29">
+      <c r="R7" s="54">
         <v>7.9833333333333334</v>
       </c>
-      <c r="S7" s="35">
+      <c r="S7" s="55">
         <v>18554666.666666668</v>
       </c>
-      <c r="T7" s="28">
-        <v>6350.2059162417154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T7" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="U7" s="56">
+        <v>7.983333333</v>
+      </c>
+      <c r="V7" s="57" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>76</v>
       </c>
@@ -15259,20 +16639,26 @@
       <c r="D8" s="29">
         <v>4214.8956770102141</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q8" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="R8" s="29">
+      <c r="R8" s="54">
         <v>23.720765027322404</v>
       </c>
-      <c r="S8" s="35">
+      <c r="S8" s="55">
         <v>76264666.666666672</v>
       </c>
-      <c r="T8" s="28">
-        <v>8784.430264077344</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T8" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="U8" s="56">
+        <v>23.720765029999999</v>
+      </c>
+      <c r="V8" s="57" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>90</v>
       </c>
@@ -15294,11 +16680,17 @@
       <c r="S9" s="35">
         <v>968752819.45899999</v>
       </c>
-      <c r="T9" s="27">
-        <v>21068.728733090302</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T9" t="s">
+        <v>111</v>
+      </c>
+      <c r="U9">
+        <v>125.63005870000001</v>
+      </c>
+      <c r="V9" s="35">
+        <v>968752819.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>90</v>
       </c>
@@ -15320,11 +16712,17 @@
       <c r="S10" s="35">
         <v>206329392</v>
       </c>
-      <c r="T10" s="28">
-        <v>15785.702470802906</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T10" t="s">
+        <v>118</v>
+      </c>
+      <c r="U10">
+        <v>35.712158469999999</v>
+      </c>
+      <c r="V10" s="35">
+        <v>206329392</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>90</v>
       </c>
@@ -15346,11 +16744,17 @@
       <c r="S11" s="35">
         <v>121391220</v>
       </c>
-      <c r="T11" s="28">
-        <v>11575.510398687888</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T11" t="s">
+        <v>121</v>
+      </c>
+      <c r="U11">
+        <v>28.652732239999999</v>
+      </c>
+      <c r="V11" s="35">
+        <v>121391220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>111</v>
       </c>
@@ -15372,11 +16776,17 @@
       <c r="S12" s="35">
         <v>78667674</v>
       </c>
-      <c r="T12" s="28">
-        <v>11326.73329196249</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T12" t="s">
+        <v>121</v>
+      </c>
+      <c r="U12">
+        <v>18.976256830000001</v>
+      </c>
+      <c r="V12" s="35">
+        <v>78667674</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>118</v>
       </c>
@@ -15398,11 +16808,17 @@
       <c r="S13" s="35">
         <v>29680770</v>
       </c>
-      <c r="T13" s="28">
-        <v>12786.160460427687</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T13" t="s">
+        <v>121</v>
+      </c>
+      <c r="U13">
+        <v>6.3424043719999998</v>
+      </c>
+      <c r="V13" s="35">
+        <v>29680770</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>121</v>
       </c>
@@ -15424,11 +16840,17 @@
       <c r="S14" s="35">
         <v>159260997.59999999</v>
       </c>
-      <c r="T14" s="28">
-        <v>10476.063103201592</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T14" t="s">
+        <v>127</v>
+      </c>
+      <c r="U14">
+        <v>41.536532700000002</v>
+      </c>
+      <c r="V14" s="35">
+        <v>159260997.59999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>121</v>
       </c>
@@ -15450,11 +16872,17 @@
       <c r="S15" s="35">
         <v>51331878</v>
       </c>
-      <c r="T15" s="28">
-        <v>11696.70747338259</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T15" t="s">
+        <v>130</v>
+      </c>
+      <c r="U15">
+        <v>11.990642080000001</v>
+      </c>
+      <c r="V15" s="35">
+        <v>51331878</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>121</v>
       </c>
@@ -15476,11 +16904,17 @@
       <c r="S16" s="35">
         <v>284977500</v>
       </c>
-      <c r="T16" s="28">
-        <v>16582.53517520686</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T16" t="s">
+        <v>136</v>
+      </c>
+      <c r="U16">
+        <v>46.954644809999998</v>
+      </c>
+      <c r="V16" s="35">
+        <v>284977500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>127</v>
       </c>
@@ -15502,11 +16936,17 @@
       <c r="S17" s="35">
         <v>3709528</v>
       </c>
-      <c r="T17" s="28">
-        <v>6748.8911125261529</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T17" t="s">
+        <v>142</v>
+      </c>
+      <c r="U17">
+        <v>1.5017759559999999</v>
+      </c>
+      <c r="V17" s="35">
+        <v>3709528</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>130</v>
       </c>
@@ -15528,11 +16968,17 @@
       <c r="S18" s="35">
         <v>22284115</v>
       </c>
-      <c r="T18" s="28">
-        <v>16213.232298245102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T18" t="s">
+        <v>142</v>
+      </c>
+      <c r="U18">
+        <v>3.755300546</v>
+      </c>
+      <c r="V18" s="35">
+        <v>22284115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>136</v>
       </c>
@@ -15554,11 +17000,17 @@
       <c r="S19" s="35">
         <v>38351800</v>
       </c>
-      <c r="T19" s="28">
-        <v>19843.227749205791</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T19" t="s">
+        <v>142</v>
+      </c>
+      <c r="U19">
+        <v>5.2807103829999997</v>
+      </c>
+      <c r="V19" s="35">
+        <v>38351800</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>142</v>
       </c>
@@ -15580,11 +17032,17 @@
       <c r="S20" s="35">
         <v>236718970</v>
       </c>
-      <c r="T20" s="28">
-        <v>16409.075911022384</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T20" t="s">
+        <v>167</v>
+      </c>
+      <c r="U20">
+        <v>39.415573770000002</v>
+      </c>
+      <c r="V20" s="35">
+        <v>236718970</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>142</v>
       </c>
@@ -15606,11 +17064,17 @@
       <c r="S21" s="35">
         <v>133967709.40000001</v>
       </c>
-      <c r="T21" s="28">
-        <v>15399.313497740444</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T21" t="s">
+        <v>170</v>
+      </c>
+      <c r="U21">
+        <v>23.769370819999999</v>
+      </c>
+      <c r="V21" s="35">
+        <v>133967709.40000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>142</v>
       </c>
@@ -15632,11 +17096,17 @@
       <c r="S22" s="35">
         <v>6468208.7000000002</v>
       </c>
-      <c r="T22" s="28">
-        <v>7859.0314633146982</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T22" t="s">
+        <v>170</v>
+      </c>
+      <c r="U22">
+        <v>2.248712383</v>
+      </c>
+      <c r="V22" s="35">
+        <v>6468208.7000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="29"/>
       <c r="C23" s="35"/>
@@ -15650,11 +17120,17 @@
       <c r="S23" s="35">
         <v>415332388.10000002</v>
       </c>
-      <c r="T23" s="28">
-        <v>10879.986527472378</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T23" t="s">
+        <v>182</v>
+      </c>
+      <c r="U23">
+        <v>104.3004918</v>
+      </c>
+      <c r="V23" s="35">
+        <v>415332388.10000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>167</v>
       </c>
@@ -15676,11 +17152,17 @@
       <c r="S24" s="35">
         <v>331468584.19999999</v>
       </c>
-      <c r="T24" s="28">
-        <v>24716.645766755799</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T24" t="s">
+        <v>188</v>
+      </c>
+      <c r="U24">
+        <v>36.641374319999997</v>
+      </c>
+      <c r="V24" s="35">
+        <v>331468584.19999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>170</v>
       </c>
@@ -15702,11 +17184,17 @@
       <c r="S25" s="35">
         <v>331360000</v>
       </c>
-      <c r="T25" s="28">
-        <v>24691.505216095378</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T25" t="s">
+        <v>188</v>
+      </c>
+      <c r="U25">
+        <v>36.666666669999998</v>
+      </c>
+      <c r="V25" s="35">
+        <v>331360000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>170</v>
       </c>
@@ -15728,11 +17216,17 @@
       <c r="S26" s="35">
         <v>338700000</v>
       </c>
-      <c r="T26" s="28">
-        <v>11628.425956761619</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T26" t="s">
+        <v>196</v>
+      </c>
+      <c r="U26">
+        <v>79.581693990000005</v>
+      </c>
+      <c r="V26" s="35">
+        <v>338700000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>182</v>
       </c>
@@ -15745,20 +17239,26 @@
       <c r="D27" s="28">
         <v>10879.986527472378</v>
       </c>
-      <c r="Q27" s="23" t="s">
+      <c r="Q27" s="53" t="s">
         <v>201</v>
       </c>
-      <c r="R27" s="30">
+      <c r="R27" s="54">
         <v>156.51639344262296</v>
       </c>
-      <c r="S27" s="35">
+      <c r="S27" s="55">
         <v>213348333.33333337</v>
       </c>
-      <c r="T27" s="27">
-        <v>3724.331558581363</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T27" s="56" t="s">
+        <v>201</v>
+      </c>
+      <c r="U27" s="56">
+        <v>156.5163934</v>
+      </c>
+      <c r="V27" s="57" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>188</v>
       </c>
@@ -15780,11 +17280,17 @@
       <c r="S28" s="35">
         <v>132875000</v>
       </c>
-      <c r="T28" s="28">
-        <v>4480.1371874482656</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T28" t="s">
+        <v>228</v>
+      </c>
+      <c r="U28">
+        <v>81.034672130000004</v>
+      </c>
+      <c r="V28" s="35">
+        <v>132875000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>188</v>
       </c>
@@ -15806,11 +17312,17 @@
       <c r="S29" s="35">
         <v>100610000</v>
       </c>
-      <c r="T29" s="28">
-        <v>3930.9994529967962</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T29" t="s">
+        <v>235</v>
+      </c>
+      <c r="U29">
+        <v>69.928961749999999</v>
+      </c>
+      <c r="V29" s="35">
+        <v>100610000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>196</v>
       </c>
@@ -15832,11 +17344,17 @@
       <c r="S30" s="35">
         <v>47796306</v>
       </c>
-      <c r="T30" s="28">
-        <v>10182.534113060428</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T30" t="s">
+        <v>252</v>
+      </c>
+      <c r="U30">
+        <v>12.824999999999999</v>
+      </c>
+      <c r="V30" s="35">
+        <v>47796306</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
         <v>196</v>
       </c>
@@ -15858,11 +17376,17 @@
       <c r="S31" s="35">
         <v>260120703.40000001</v>
       </c>
-      <c r="T31" s="28">
-        <v>26597.10015500959</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T31" t="s">
+        <v>255</v>
+      </c>
+      <c r="U31">
+        <v>26.721420770000002</v>
+      </c>
+      <c r="V31" s="35">
+        <v>260120703.40000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
         <v>201</v>
       </c>
@@ -15884,11 +17408,17 @@
       <c r="S32" s="35">
         <v>1054080000</v>
       </c>
-      <c r="T32" s="28">
-        <v>20065.331109943578</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T32" t="s">
+        <v>259</v>
+      </c>
+      <c r="U32">
+        <v>143.5311475</v>
+      </c>
+      <c r="V32" s="35">
+        <v>1054080000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="29"/>
       <c r="C33" s="35"/>
@@ -15902,11 +17432,17 @@
       <c r="S33" s="35">
         <v>109251549</v>
       </c>
-      <c r="T33" s="28">
-        <v>9820.2138933607312</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T33" t="s">
+        <v>265</v>
+      </c>
+      <c r="U33">
+        <v>30.39663934</v>
+      </c>
+      <c r="V33" s="35">
+        <v>109251549</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>222</v>
       </c>
@@ -15928,11 +17464,17 @@
       <c r="S34" s="35">
         <v>230512400</v>
       </c>
-      <c r="T34" s="28">
-        <v>4285.0033878518789</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T34" t="s">
+        <v>271</v>
+      </c>
+      <c r="U34">
+        <v>146.9812842</v>
+      </c>
+      <c r="V34" s="35">
+        <v>230512400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>228</v>
       </c>
@@ -15945,20 +17487,26 @@
       <c r="D35" s="28">
         <v>4480.1371874482656</v>
       </c>
-      <c r="Q35" s="2" t="s">
+      <c r="Q35" s="53" t="s">
         <v>281</v>
       </c>
-      <c r="R35" s="29">
+      <c r="R35" s="54">
         <v>107.19683057377048</v>
       </c>
-      <c r="S35" s="35">
+      <c r="S35" s="55">
         <v>515209333.33333337</v>
       </c>
-      <c r="T35" s="28">
-        <v>13131.69210880782</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T35" s="56" t="s">
+        <v>281</v>
+      </c>
+      <c r="U35" s="56">
+        <v>107.1968306</v>
+      </c>
+      <c r="V35" s="57" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>235</v>
       </c>
@@ -15980,11 +17528,17 @@
       <c r="S36" s="35">
         <v>22684790</v>
       </c>
-      <c r="T36" s="28">
-        <v>10730.211740705734</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T36" t="s">
+        <v>284</v>
+      </c>
+      <c r="U36">
+        <v>5.776242077</v>
+      </c>
+      <c r="V36" s="35">
+        <v>22684790</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>252</v>
       </c>
@@ -16006,11 +17560,17 @@
       <c r="S37" s="35">
         <v>525983532</v>
       </c>
-      <c r="T37" s="28">
-        <v>14062.283214161109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T37" t="s">
+        <v>288</v>
+      </c>
+      <c r="U37">
+        <v>102.19631149999999</v>
+      </c>
+      <c r="V37" s="35">
+        <v>525983532</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>255</v>
       </c>
@@ -16023,20 +17583,26 @@
       <c r="D38" s="28">
         <v>26597.10015500959</v>
       </c>
-      <c r="Q38" s="2" t="s">
+      <c r="Q38" s="53" t="s">
         <v>296</v>
       </c>
-      <c r="R38" s="29">
+      <c r="R38" s="54">
         <v>33.748770491803278</v>
       </c>
-      <c r="S38" s="35">
+      <c r="S38" s="55">
         <v>229510953.33333334</v>
       </c>
-      <c r="T38" s="28">
-        <v>18580.798598883048</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T38" s="56" t="s">
+        <v>296</v>
+      </c>
+      <c r="U38" s="56">
+        <v>33.748770489999998</v>
+      </c>
+      <c r="V38" s="57" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>259</v>
       </c>
@@ -16058,11 +17624,17 @@
       <c r="S39" s="35">
         <v>198866597</v>
       </c>
-      <c r="T39" s="28">
-        <v>9498.9681212862306</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T39" t="s">
+        <v>302</v>
+      </c>
+      <c r="U39">
+        <v>57.201092899999999</v>
+      </c>
+      <c r="V39" s="35">
+        <v>198866597</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>265</v>
       </c>
@@ -16084,11 +17656,17 @@
       <c r="S40" s="35">
         <v>12270048</v>
       </c>
-      <c r="T40" s="28">
-        <v>14194.708529517244</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T40" t="s">
+        <v>302</v>
+      </c>
+      <c r="U40">
+        <v>2.3617759559999998</v>
+      </c>
+      <c r="V40" s="35">
+        <v>12270048</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>271</v>
       </c>
@@ -16110,11 +17688,17 @@
       <c r="S41" s="35">
         <v>222437605</v>
       </c>
-      <c r="T41" s="28">
-        <v>10195.141855348795</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T41" t="s">
+        <v>317</v>
+      </c>
+      <c r="U41">
+        <v>59.612021859999999</v>
+      </c>
+      <c r="V41" s="35">
+        <v>222437605</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>281</v>
       </c>
@@ -16127,20 +17711,26 @@
       <c r="D42" s="28">
         <v>13131.69210880782</v>
       </c>
-      <c r="Q42" s="2" t="s">
+      <c r="Q42" s="53" t="s">
         <v>328</v>
       </c>
-      <c r="R42" s="29">
+      <c r="R42" s="54">
         <v>22.460655737704919</v>
       </c>
-      <c r="S42" s="35">
+      <c r="S42" s="55">
         <v>76583333.333333343</v>
       </c>
-      <c r="T42" s="28">
-        <v>9316.0272161804896</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="T42" s="56" t="s">
+        <v>328</v>
+      </c>
+      <c r="U42" s="56">
+        <v>22.46065574</v>
+      </c>
+      <c r="V42" s="55">
+        <v>70692307.692307696</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>284</v>
       </c>
@@ -16153,20 +17743,26 @@
       <c r="D43" s="28">
         <v>10730.211740705734</v>
       </c>
-      <c r="Q43" s="2" t="s">
+      <c r="Q43" s="53" t="s">
         <v>328</v>
       </c>
-      <c r="R43" s="29">
+      <c r="R43" s="54">
         <v>33.089344262295086</v>
       </c>
-      <c r="S43" s="35">
+      <c r="S43" s="55">
         <v>20184500.000000004</v>
       </c>
-      <c r="T43" s="28">
-        <v>1666.666666666667</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T43" s="56" t="s">
+        <v>328</v>
+      </c>
+      <c r="U43" s="56">
+        <v>33.089344259999997</v>
+      </c>
+      <c r="V43" s="57" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>288</v>
       </c>
@@ -16180,7 +17776,7 @@
         <v>14062.283214161109</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>296</v>
       </c>
@@ -16194,7 +17790,7 @@
         <v>18580.798598883048</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>302</v>
       </c>
@@ -16208,7 +17804,7 @@
         <v>9498.9681212862306</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>302</v>
       </c>
@@ -16222,7 +17818,7 @@
         <v>14194.708529517244</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>317</v>
       </c>

</xml_diff>